<commit_message>
Generate Errors.txt BEFORE applying special rules.
</commit_message>
<xml_diff>
--- a/referenceDocsMetrics.xlsx
+++ b/referenceDocsMetrics.xlsx
@@ -118,11 +118,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Accent1" xfId="1" builtinId="29"/>
@@ -428,7 +427,7 @@
   <dimension ref="A1:R5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M10" sqref="M10"/>
+      <selection activeCell="A5" sqref="A5:XFD5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -676,59 +675,59 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>42860</v>
       </c>
-      <c r="B5" s="3">
+      <c r="B5">
         <v>229</v>
       </c>
-      <c r="C5" s="3">
+      <c r="C5">
         <v>309</v>
       </c>
-      <c r="D5" s="3">
+      <c r="D5">
         <v>67</v>
       </c>
-      <c r="E5" s="3">
+      <c r="E5">
         <v>3555</v>
       </c>
-      <c r="F5" s="3">
+      <c r="F5">
         <v>3</v>
       </c>
-      <c r="G5" s="3">
-        <v>192</v>
-      </c>
-      <c r="H5" s="3">
+      <c r="G5">
+        <v>202</v>
+      </c>
+      <c r="H5">
         <v>216</v>
       </c>
-      <c r="I5" s="3">
+      <c r="I5">
         <v>657</v>
       </c>
-      <c r="J5" s="3">
+      <c r="J5">
         <v>130</v>
       </c>
-      <c r="K5" s="3">
+      <c r="K5">
         <v>1</v>
       </c>
-      <c r="L5" s="3">
-        <v>224</v>
-      </c>
-      <c r="M5" s="3">
-        <v>10</v>
-      </c>
-      <c r="N5" s="3">
+      <c r="L5">
+        <v>225</v>
+      </c>
+      <c r="M5">
+        <v>10</v>
+      </c>
+      <c r="N5">
         <v>0</v>
       </c>
-      <c r="O5" s="3">
-        <v>10</v>
-      </c>
-      <c r="P5" s="3">
+      <c r="O5">
+        <v>10</v>
+      </c>
+      <c r="P5">
         <v>83</v>
       </c>
-      <c r="Q5" s="3">
+      <c r="Q5">
         <v>15</v>
       </c>
-      <c r="R5" s="3">
+      <c r="R5">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
SNAPSHOT_v11.1d_2017-05-06 - readonly imlemented
</commit_message>
<xml_diff>
--- a/referenceDocsMetrics.xlsx
+++ b/referenceDocsMetrics.xlsx
@@ -424,10 +424,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R5"/>
+  <dimension ref="A1:R6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:XFD5"/>
+      <selection activeCell="A6" sqref="A6:R6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -728,6 +728,62 @@
         <v>15</v>
       </c>
       <c r="R5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>42861</v>
+      </c>
+      <c r="B6">
+        <v>229</v>
+      </c>
+      <c r="C6">
+        <v>309</v>
+      </c>
+      <c r="D6">
+        <v>67</v>
+      </c>
+      <c r="E6">
+        <v>3555</v>
+      </c>
+      <c r="F6">
+        <v>3</v>
+      </c>
+      <c r="G6">
+        <v>202</v>
+      </c>
+      <c r="H6">
+        <v>216</v>
+      </c>
+      <c r="I6">
+        <v>657</v>
+      </c>
+      <c r="J6">
+        <v>130</v>
+      </c>
+      <c r="K6">
+        <v>1</v>
+      </c>
+      <c r="L6">
+        <v>225</v>
+      </c>
+      <c r="M6">
+        <v>10</v>
+      </c>
+      <c r="N6">
+        <v>0</v>
+      </c>
+      <c r="O6">
+        <v>10</v>
+      </c>
+      <c r="P6">
+        <v>83</v>
+      </c>
+      <c r="Q6">
+        <v>15</v>
+      </c>
+      <c r="R6">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Move validations. Enforce use of getters and setters.
</commit_message>
<xml_diff>
--- a/referenceDocsMetrics.xlsx
+++ b/referenceDocsMetrics.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="120" windowWidth="22995" windowHeight="9015"/>
+    <workbookView xWindow="0" yWindow="120" windowWidth="22995" windowHeight="9015" tabRatio="429"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t>Date</t>
   </si>
@@ -70,13 +70,28 @@
   </si>
   <si>
     <t>Method params with bad name</t>
+  </si>
+  <si>
+    <t>Method params missing type</t>
+  </si>
+  <si>
+    <t>Methods with required parameters after optional parameters</t>
+  </si>
+  <si>
+    <t>Setter Methods with paramter type that does not match the attribute type</t>
+  </si>
+  <si>
+    <t>Non-optional params with the word 'Optional' in the description</t>
+  </si>
+  <si>
+    <t>Getter Methods with return type that does not match the attribute type</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -85,6 +100,14 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="0"/>
       <name val="Calibri"/>
@@ -118,10 +141,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Accent1" xfId="1" builtinId="29"/>
@@ -424,371 +454,391 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R6"/>
+  <dimension ref="A1:W6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:R6"/>
+      <selection activeCell="A7" sqref="A7:XFD7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="22" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="27.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="23.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="26.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="23.28515625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="7.7109375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="8" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="28.140625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="32.5703125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="29" bestFit="1" customWidth="1"/>
+    <col min="1" max="19" width="8.7109375" style="3"/>
+    <col min="20" max="20" width="17.5703125" style="3" customWidth="1"/>
+    <col min="21" max="21" width="15.140625" style="3" customWidth="1"/>
+    <col min="22" max="22" width="17.140625" style="3" customWidth="1"/>
+    <col min="23" max="23" width="16.42578125" style="3" customWidth="1"/>
+    <col min="24" max="16384" width="8.7109375" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:23" s="1" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="J1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" s="2" t="s">
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="M1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="N1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="2" t="s">
+      <c r="O1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="2" t="s">
+      <c r="P1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="2" t="s">
+      <c r="Q1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="2" t="s">
+      <c r="R1" s="1" t="s">
         <v>17</v>
       </c>
+      <c r="S1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>22</v>
+      </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A2" s="1">
+    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A2" s="2">
         <v>42856</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="3">
         <v>229</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="3">
         <v>309</v>
       </c>
-      <c r="D2">
+      <c r="D2" s="3">
         <v>67</v>
       </c>
-      <c r="E2">
+      <c r="E2" s="3">
         <v>3064</v>
       </c>
-      <c r="F2">
+      <c r="F2" s="3">
         <v>3</v>
       </c>
-      <c r="G2">
+      <c r="G2" s="3">
         <v>192</v>
       </c>
-      <c r="H2">
+      <c r="H2" s="3">
         <v>216</v>
       </c>
-      <c r="I2">
+      <c r="I2" s="3">
         <v>657</v>
       </c>
-      <c r="J2">
+      <c r="J2" s="3">
         <v>130</v>
       </c>
-      <c r="K2">
+      <c r="K2" s="3">
         <v>1</v>
       </c>
-      <c r="L2">
+      <c r="L2" s="3">
         <v>224</v>
       </c>
-      <c r="M2">
-        <v>10</v>
-      </c>
-      <c r="N2">
+      <c r="M2" s="3">
+        <v>10</v>
+      </c>
+      <c r="N2" s="3">
         <v>0</v>
       </c>
-      <c r="O2">
-        <v>10</v>
-      </c>
-      <c r="P2">
+      <c r="O2" s="3">
+        <v>10</v>
+      </c>
+      <c r="P2" s="3">
         <v>84</v>
       </c>
-      <c r="Q2">
+      <c r="Q2" s="3">
         <v>15</v>
       </c>
-      <c r="R2">
+      <c r="R2" s="3">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A3" s="1">
+    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A3" s="2">
         <v>42858</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="3">
         <v>229</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="3">
         <v>309</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="3">
         <v>67</v>
       </c>
-      <c r="E3">
+      <c r="E3" s="3">
         <v>3554</v>
       </c>
-      <c r="F3">
+      <c r="F3" s="3">
         <v>3</v>
       </c>
-      <c r="G3">
+      <c r="G3" s="3">
         <v>192</v>
       </c>
-      <c r="H3">
+      <c r="H3" s="3">
         <v>216</v>
       </c>
-      <c r="I3">
+      <c r="I3" s="3">
         <v>657</v>
       </c>
-      <c r="J3">
+      <c r="J3" s="3">
         <v>130</v>
       </c>
-      <c r="K3">
+      <c r="K3" s="3">
         <v>1</v>
       </c>
-      <c r="L3">
+      <c r="L3" s="3">
         <v>224</v>
       </c>
-      <c r="M3">
-        <v>10</v>
-      </c>
-      <c r="N3">
+      <c r="M3" s="3">
+        <v>10</v>
+      </c>
+      <c r="N3" s="3">
         <v>0</v>
       </c>
-      <c r="O3">
-        <v>10</v>
-      </c>
-      <c r="P3">
+      <c r="O3" s="3">
+        <v>10</v>
+      </c>
+      <c r="P3" s="3">
         <v>83</v>
       </c>
-      <c r="Q3">
+      <c r="Q3" s="3">
         <v>15</v>
       </c>
-      <c r="R3">
+      <c r="R3" s="3">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A4" s="1">
+    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A4" s="2">
         <v>42859</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="3">
         <v>229</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="3">
         <v>309</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="3">
         <v>67</v>
       </c>
-      <c r="E4">
+      <c r="E4" s="3">
         <v>3554</v>
       </c>
-      <c r="F4">
+      <c r="F4" s="3">
         <v>3</v>
       </c>
-      <c r="G4">
+      <c r="G4" s="3">
         <v>192</v>
       </c>
-      <c r="H4">
+      <c r="H4" s="3">
         <v>216</v>
       </c>
-      <c r="I4">
+      <c r="I4" s="3">
         <v>657</v>
       </c>
-      <c r="J4">
+      <c r="J4" s="3">
         <v>130</v>
       </c>
-      <c r="K4">
+      <c r="K4" s="3">
         <v>1</v>
       </c>
-      <c r="L4">
+      <c r="L4" s="3">
         <v>224</v>
       </c>
-      <c r="M4">
-        <v>10</v>
-      </c>
-      <c r="N4">
+      <c r="M4" s="3">
+        <v>10</v>
+      </c>
+      <c r="N4" s="3">
         <v>0</v>
       </c>
-      <c r="O4">
-        <v>10</v>
-      </c>
-      <c r="P4">
+      <c r="O4" s="3">
+        <v>10</v>
+      </c>
+      <c r="P4" s="3">
         <v>83</v>
       </c>
-      <c r="Q4">
+      <c r="Q4" s="3">
         <v>15</v>
       </c>
-      <c r="R4">
+      <c r="R4" s="3">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A5" s="1">
+    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A5" s="2">
         <v>42860</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="3">
         <v>229</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="3">
         <v>309</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="3">
         <v>67</v>
       </c>
-      <c r="E5">
+      <c r="E5" s="3">
         <v>3555</v>
       </c>
-      <c r="F5">
+      <c r="F5" s="3">
         <v>3</v>
       </c>
-      <c r="G5">
+      <c r="G5" s="3">
         <v>202</v>
       </c>
-      <c r="H5">
+      <c r="H5" s="3">
         <v>216</v>
       </c>
-      <c r="I5">
+      <c r="I5" s="3">
         <v>657</v>
       </c>
-      <c r="J5">
+      <c r="J5" s="3">
         <v>130</v>
       </c>
-      <c r="K5">
+      <c r="K5" s="3">
         <v>1</v>
       </c>
-      <c r="L5">
+      <c r="L5" s="3">
         <v>225</v>
       </c>
-      <c r="M5">
-        <v>10</v>
-      </c>
-      <c r="N5">
+      <c r="M5" s="3">
+        <v>10</v>
+      </c>
+      <c r="N5" s="3">
         <v>0</v>
       </c>
-      <c r="O5">
-        <v>10</v>
-      </c>
-      <c r="P5">
+      <c r="O5" s="3">
+        <v>10</v>
+      </c>
+      <c r="P5" s="3">
         <v>83</v>
       </c>
-      <c r="Q5">
+      <c r="Q5" s="3">
         <v>15</v>
       </c>
-      <c r="R5">
+      <c r="R5" s="3">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A6" s="1">
+    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A6" s="2">
         <v>42861</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="3">
         <v>229</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="3">
         <v>309</v>
       </c>
-      <c r="D6">
+      <c r="D6" s="3">
         <v>67</v>
       </c>
-      <c r="E6">
+      <c r="E6" s="3">
         <v>3555</v>
       </c>
-      <c r="F6">
+      <c r="F6" s="3">
         <v>3</v>
       </c>
-      <c r="G6">
+      <c r="G6" s="3">
         <v>202</v>
       </c>
-      <c r="H6">
+      <c r="H6" s="3">
         <v>216</v>
       </c>
-      <c r="I6">
+      <c r="I6" s="3">
         <v>657</v>
       </c>
-      <c r="J6">
+      <c r="J6" s="3">
         <v>130</v>
       </c>
-      <c r="K6">
+      <c r="K6" s="3">
         <v>1</v>
       </c>
-      <c r="L6">
+      <c r="L6" s="3">
         <v>225</v>
       </c>
-      <c r="M6">
-        <v>10</v>
-      </c>
-      <c r="N6">
+      <c r="M6" s="3">
+        <v>10</v>
+      </c>
+      <c r="N6" s="3">
         <v>0</v>
       </c>
-      <c r="O6">
-        <v>10</v>
-      </c>
-      <c r="P6">
+      <c r="O6" s="3">
+        <v>10</v>
+      </c>
+      <c r="P6" s="3">
         <v>83</v>
       </c>
-      <c r="Q6">
+      <c r="Q6" s="3">
         <v>15</v>
       </c>
-      <c r="R6">
+      <c r="R6" s="3">
         <v>1</v>
+      </c>
+      <c r="S6" s="3">
+        <v>7</v>
+      </c>
+      <c r="T6" s="3">
+        <v>7</v>
+      </c>
+      <c r="U6" s="3">
+        <v>88</v>
+      </c>
+      <c r="V6" s="3">
+        <v>19</v>
+      </c>
+      <c r="W6" s="3">
+        <v>42</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
SNAPSHOT_v11.1d_2017-05-09. Minor fixed in progress report.
</commit_message>
<xml_diff>
--- a/referenceDocsMetrics.xlsx
+++ b/referenceDocsMetrics.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
   <si>
     <t>Date</t>
   </si>
@@ -85,13 +85,43 @@
   </si>
   <si>
     <t>Getter Methods with return type that does not match the attribute type</t>
+  </si>
+  <si>
+    <t>Types Generated</t>
+  </si>
+  <si>
+    <t>Interfaces Generated</t>
+  </si>
+  <si>
+    <t>Objects Generated</t>
+  </si>
+  <si>
+    <t>Classes Generated</t>
+  </si>
+  <si>
+    <t>Generated Methods</t>
+  </si>
+  <si>
+    <t>Percentage of Types generated</t>
+  </si>
+  <si>
+    <t>Percentage of Interfaces generated</t>
+  </si>
+  <si>
+    <t>Percentage of Objects generated</t>
+  </si>
+  <si>
+    <t>Percentage of Classes generated</t>
+  </si>
+  <si>
+    <t>Percentage of Methods generated</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -110,6 +140,13 @@
       <b/>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -137,11 +174,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -152,10 +190,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="9" fontId="2" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
     <cellStyle name="Accent1" xfId="1" builtinId="29"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="2" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -454,10 +499,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:W6"/>
+  <dimension ref="A1:AG7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7:XFD7"/>
+    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
+      <selection activeCell="AB11" sqref="AB11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -467,10 +512,20 @@
     <col min="21" max="21" width="15.140625" style="3" customWidth="1"/>
     <col min="22" max="22" width="17.140625" style="3" customWidth="1"/>
     <col min="23" max="23" width="16.42578125" style="3" customWidth="1"/>
-    <col min="24" max="16384" width="8.7109375" style="3"/>
+    <col min="24" max="24" width="12.7109375" style="3" customWidth="1"/>
+    <col min="25" max="25" width="11.42578125" style="3" customWidth="1"/>
+    <col min="26" max="26" width="11.28515625" style="3" customWidth="1"/>
+    <col min="27" max="27" width="12.140625" style="3" customWidth="1"/>
+    <col min="28" max="28" width="12.28515625" style="3" customWidth="1"/>
+    <col min="29" max="29" width="13.28515625" style="3" customWidth="1"/>
+    <col min="30" max="30" width="15.85546875" style="5" customWidth="1"/>
+    <col min="31" max="31" width="15" style="5" customWidth="1"/>
+    <col min="32" max="32" width="14.42578125" style="5" customWidth="1"/>
+    <col min="33" max="33" width="13.85546875" style="5" customWidth="1"/>
+    <col min="34" max="16384" width="8.7109375" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" s="1" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:33" s="1" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -540,8 +595,38 @@
       <c r="W1" s="1" t="s">
         <v>22</v>
       </c>
+      <c r="X1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="Y1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="Z1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="AA1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="AB1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="AC1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="AD1" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="AE1" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="AF1" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="AG1" s="4" t="s">
+        <v>32</v>
+      </c>
     </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>42856</v>
       </c>
@@ -597,7 +682,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>42858</v>
       </c>
@@ -653,7 +738,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>42859</v>
       </c>
@@ -709,7 +794,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>42860</v>
       </c>
@@ -765,7 +850,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>42861</v>
       </c>
@@ -834,6 +919,107 @@
       </c>
       <c r="W6" s="3">
         <v>42</v>
+      </c>
+    </row>
+    <row r="7" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A7" s="2">
+        <v>42864</v>
+      </c>
+      <c r="B7" s="3">
+        <v>229</v>
+      </c>
+      <c r="C7" s="3">
+        <v>309</v>
+      </c>
+      <c r="D7" s="3">
+        <v>67</v>
+      </c>
+      <c r="E7" s="3">
+        <v>3555</v>
+      </c>
+      <c r="F7" s="3">
+        <v>3</v>
+      </c>
+      <c r="G7" s="3">
+        <v>202</v>
+      </c>
+      <c r="H7" s="3">
+        <v>216</v>
+      </c>
+      <c r="I7" s="3">
+        <v>657</v>
+      </c>
+      <c r="J7" s="3">
+        <v>130</v>
+      </c>
+      <c r="K7" s="3">
+        <v>1</v>
+      </c>
+      <c r="L7" s="3">
+        <v>225</v>
+      </c>
+      <c r="M7" s="3">
+        <v>10</v>
+      </c>
+      <c r="N7" s="3">
+        <v>0</v>
+      </c>
+      <c r="O7" s="3">
+        <v>10</v>
+      </c>
+      <c r="P7" s="3">
+        <v>83</v>
+      </c>
+      <c r="Q7" s="3">
+        <v>15</v>
+      </c>
+      <c r="R7" s="3">
+        <v>1</v>
+      </c>
+      <c r="S7" s="3">
+        <v>7</v>
+      </c>
+      <c r="T7" s="3">
+        <v>7</v>
+      </c>
+      <c r="U7" s="3">
+        <v>88</v>
+      </c>
+      <c r="V7" s="3">
+        <v>19</v>
+      </c>
+      <c r="W7" s="3">
+        <v>42</v>
+      </c>
+      <c r="X7" s="3">
+        <v>229</v>
+      </c>
+      <c r="Y7" s="3">
+        <v>3</v>
+      </c>
+      <c r="Z7" s="3">
+        <v>25</v>
+      </c>
+      <c r="AA7" s="3">
+        <v>77</v>
+      </c>
+      <c r="AB7" s="3">
+        <v>353</v>
+      </c>
+      <c r="AC7" s="3">
+        <v>1</v>
+      </c>
+      <c r="AD7" s="5">
+        <v>0.6</v>
+      </c>
+      <c r="AE7" s="5">
+        <v>0.37313429999999997</v>
+      </c>
+      <c r="AF7" s="5">
+        <v>0.24919089999999999</v>
+      </c>
+      <c r="AG7" s="5">
+        <v>9.9296759999999998E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
SNAPSHOT_v11.1d_2017-05-10. Added DEPRECATED and @deprecated tags appropriately, added @return tags, added interfaces file, better formatted descriptions, refined validation rules, generated more interfaces, classes, objects and methods.
</commit_message>
<xml_diff>
--- a/referenceDocsMetrics.xlsx
+++ b/referenceDocsMetrics.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="120" windowWidth="22995" windowHeight="9015" tabRatio="429"/>
+    <workbookView xWindow="0" yWindow="120" windowWidth="22995" windowHeight="8280" tabRatio="230"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -523,15 +523,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AL7"/>
+  <dimension ref="A1:AL8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AM10" sqref="AM10"/>
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="8.7109375" style="3"/>
+    <col min="1" max="1" width="9.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.7109375" style="3"/>
     <col min="3" max="3" width="10.140625" style="3" customWidth="1"/>
     <col min="4" max="6" width="8.7109375" style="3"/>
     <col min="7" max="7" width="10.7109375" style="3" customWidth="1"/>
@@ -1102,6 +1103,122 @@
       </c>
       <c r="AL7" s="5">
         <v>9.9296759999999998E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A8" s="2">
+        <v>42865</v>
+      </c>
+      <c r="B8" s="3">
+        <v>229</v>
+      </c>
+      <c r="C8" s="3">
+        <v>5</v>
+      </c>
+      <c r="D8" s="3">
+        <v>309</v>
+      </c>
+      <c r="E8" s="3">
+        <v>67</v>
+      </c>
+      <c r="F8" s="3">
+        <v>3555</v>
+      </c>
+      <c r="G8" s="3">
+        <v>3</v>
+      </c>
+      <c r="H8" s="3">
+        <v>202</v>
+      </c>
+      <c r="I8" s="3">
+        <v>216</v>
+      </c>
+      <c r="J8" s="3">
+        <v>657</v>
+      </c>
+      <c r="K8" s="3">
+        <v>130</v>
+      </c>
+      <c r="L8" s="3">
+        <v>1</v>
+      </c>
+      <c r="M8" s="3">
+        <v>225</v>
+      </c>
+      <c r="N8" s="3">
+        <v>10</v>
+      </c>
+      <c r="O8" s="3">
+        <v>0</v>
+      </c>
+      <c r="P8" s="3">
+        <v>10</v>
+      </c>
+      <c r="Q8" s="3">
+        <v>83</v>
+      </c>
+      <c r="R8" s="3">
+        <v>15</v>
+      </c>
+      <c r="S8" s="3">
+        <v>1</v>
+      </c>
+      <c r="T8" s="3">
+        <v>7</v>
+      </c>
+      <c r="U8" s="3">
+        <v>7</v>
+      </c>
+      <c r="V8" s="3">
+        <v>83</v>
+      </c>
+      <c r="W8" s="3">
+        <v>19</v>
+      </c>
+      <c r="X8" s="3">
+        <v>15</v>
+      </c>
+      <c r="Y8" s="3">
+        <v>45</v>
+      </c>
+      <c r="Z8" s="3">
+        <v>240</v>
+      </c>
+      <c r="AA8" s="3">
+        <v>130</v>
+      </c>
+      <c r="AB8" s="3">
+        <v>0</v>
+      </c>
+      <c r="AC8" s="3">
+        <v>229</v>
+      </c>
+      <c r="AD8" s="8">
+        <v>5</v>
+      </c>
+      <c r="AE8" s="8">
+        <v>30</v>
+      </c>
+      <c r="AF8" s="8">
+        <v>85</v>
+      </c>
+      <c r="AG8" s="8">
+        <v>503</v>
+      </c>
+      <c r="AH8" s="5">
+        <v>1</v>
+      </c>
+      <c r="AI8" s="5">
+        <v>1</v>
+      </c>
+      <c r="AJ8" s="5">
+        <v>0.44776120000000003</v>
+      </c>
+      <c r="AK8" s="5">
+        <v>0.27508090000000002</v>
+      </c>
+      <c r="AL8" s="5">
+        <v>0.1414909</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
SNAPSHOT_v11.1d_2017-05-12. More stuff generated.
</commit_message>
<xml_diff>
--- a/referenceDocsMetrics.xlsx
+++ b/referenceDocsMetrics.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="42">
   <si>
     <t>Date</t>
   </si>
@@ -130,6 +130,18 @@
   </si>
   <si>
     <t>Methods Generated</t>
+  </si>
+  <si>
+    <t>OR specified as ' or '</t>
+  </si>
+  <si>
+    <t>OR specified as ' | '</t>
+  </si>
+  <si>
+    <t>OR specified as ' || '</t>
+  </si>
+  <si>
+    <t>OR specified as ', '</t>
   </si>
 </sst>
 </file>
@@ -194,31 +206,40 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="9" fontId="2" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="9" fontId="2" fillId="2" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -234,6 +255,371 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$AL$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Percentage of Types generated</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$A$7:$A$8</c:f>
+              <c:numCache>
+                <c:formatCode>m/d/yyyy</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>42864</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>42865</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$AL$7:$AL$8</c:f>
+              <c:numCache>
+                <c:formatCode>0%</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$AM$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Percentage of Interfaces generated</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$A$7:$A$8</c:f>
+              <c:numCache>
+                <c:formatCode>m/d/yyyy</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>42864</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>42865</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$AM$7:$AM$8</c:f>
+              <c:numCache>
+                <c:formatCode>0%</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$AN$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Percentage of Objects generated</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="triangle"/>
+            <c:size val="5"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$A$7:$A$8</c:f>
+              <c:numCache>
+                <c:formatCode>m/d/yyyy</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>42864</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>42865</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$AN$7:$AN$8</c:f>
+              <c:numCache>
+                <c:formatCode>0%</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>0.37313429999999997</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.44776120000000003</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$AO$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Percentage of Classes generated</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$A$7:$A$8</c:f>
+              <c:numCache>
+                <c:formatCode>m/d/yyyy</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>42864</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>42865</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$AO$7:$AO$8</c:f>
+              <c:numCache>
+                <c:formatCode>0%</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>0.24919089999999999</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.27508090000000002</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$AP$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Percentage of Methods generated</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$A$7:$A$8</c:f>
+              <c:numCache>
+                <c:formatCode>m/d/yyyy</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>42864</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>42865</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$AP$7:$AP$8</c:f>
+              <c:numCache>
+                <c:formatCode>0%</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>9.9296759999999998E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.1414909</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="102020992"/>
+        <c:axId val="102022528"/>
+      </c:lineChart>
+      <c:dateAx>
+        <c:axId val="102020992"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="m/d/yyyy" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="102022528"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblOffset val="100"/>
+        <c:baseTimeUnit val="days"/>
+      </c:dateAx>
+      <c:valAx>
+        <c:axId val="102022528"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="0%" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="102020992"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>123825</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>38099</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>495300</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>9524</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -523,823 +909,898 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AL9"/>
+  <dimension ref="A1:AP9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9:XFD9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.7109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.7109375" style="3"/>
-    <col min="3" max="3" width="10.140625" style="3" customWidth="1"/>
-    <col min="4" max="6" width="8.7109375" style="3"/>
-    <col min="7" max="7" width="10.7109375" style="3" customWidth="1"/>
-    <col min="8" max="19" width="8.7109375" style="3"/>
-    <col min="20" max="20" width="11.7109375" style="3" customWidth="1"/>
-    <col min="21" max="21" width="15.140625" style="3" customWidth="1"/>
-    <col min="22" max="22" width="17.140625" style="3" customWidth="1"/>
-    <col min="23" max="23" width="16.42578125" style="3" customWidth="1"/>
-    <col min="24" max="24" width="18.28515625" style="3" customWidth="1"/>
-    <col min="25" max="25" width="11.42578125" style="3" customWidth="1"/>
-    <col min="26" max="26" width="11.28515625" style="3" customWidth="1"/>
-    <col min="27" max="27" width="12.140625" style="3" customWidth="1"/>
-    <col min="28" max="28" width="12.28515625" style="3" customWidth="1"/>
-    <col min="29" max="29" width="13.28515625" style="3" customWidth="1"/>
-    <col min="30" max="30" width="15.85546875" style="8" customWidth="1"/>
-    <col min="31" max="31" width="15" style="8" customWidth="1"/>
-    <col min="32" max="32" width="14.42578125" style="8" customWidth="1"/>
-    <col min="33" max="33" width="13.85546875" style="8" customWidth="1"/>
-    <col min="34" max="35" width="16.5703125" style="5" customWidth="1"/>
-    <col min="36" max="36" width="15.42578125" style="5" customWidth="1"/>
-    <col min="37" max="37" width="12.5703125" style="5" customWidth="1"/>
-    <col min="38" max="38" width="12.85546875" style="5" customWidth="1"/>
-    <col min="39" max="16384" width="8.7109375" style="3"/>
+    <col min="1" max="1" width="9.7109375" style="11" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.7109375" style="11"/>
+    <col min="3" max="3" width="10.140625" style="11" customWidth="1"/>
+    <col min="4" max="6" width="8.7109375" style="11"/>
+    <col min="7" max="7" width="10.7109375" style="11" customWidth="1"/>
+    <col min="8" max="19" width="8.7109375" style="11"/>
+    <col min="20" max="20" width="11.7109375" style="11" customWidth="1"/>
+    <col min="21" max="21" width="15.140625" style="11" customWidth="1"/>
+    <col min="22" max="22" width="17.140625" style="11" customWidth="1"/>
+    <col min="23" max="23" width="16.42578125" style="11" customWidth="1"/>
+    <col min="24" max="24" width="18.28515625" style="11" customWidth="1"/>
+    <col min="25" max="25" width="11.42578125" style="11" customWidth="1"/>
+    <col min="26" max="26" width="11.28515625" style="11" customWidth="1"/>
+    <col min="27" max="27" width="12.140625" style="11" customWidth="1"/>
+    <col min="28" max="28" width="12.28515625" style="11" customWidth="1"/>
+    <col min="29" max="29" width="18.140625" style="11" customWidth="1"/>
+    <col min="30" max="30" width="15.85546875" style="6" customWidth="1"/>
+    <col min="31" max="31" width="15" style="6" customWidth="1"/>
+    <col min="32" max="32" width="14.42578125" style="6" customWidth="1"/>
+    <col min="33" max="33" width="13.85546875" style="6" customWidth="1"/>
+    <col min="34" max="35" width="16.5703125" style="6" customWidth="1"/>
+    <col min="36" max="36" width="15.42578125" style="6" customWidth="1"/>
+    <col min="37" max="37" width="12.5703125" style="6" customWidth="1"/>
+    <col min="38" max="38" width="12.85546875" style="4" customWidth="1"/>
+    <col min="39" max="39" width="12.7109375" style="5" customWidth="1"/>
+    <col min="40" max="40" width="11.85546875" style="5" customWidth="1"/>
+    <col min="41" max="41" width="12.140625" style="5" customWidth="1"/>
+    <col min="42" max="42" width="11.140625" style="5" customWidth="1"/>
+    <col min="43" max="16384" width="8.7109375" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:38" s="1" customFormat="1" ht="90" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:42" s="1" customFormat="1" ht="90" x14ac:dyDescent="0.25">
+      <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J1" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="K1" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="L1" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="M1" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="N1" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="O1" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="P1" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="Q1" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="R1" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="S1" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="T1" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="U1" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="V1" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="W1" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="X1" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="Y1" s="1" t="s">
+      <c r="Y1" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="Z1" s="1" t="s">
+      <c r="Z1" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="AA1" s="1" t="s">
+      <c r="AA1" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="AB1" s="1" t="s">
+      <c r="AB1" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="AC1" s="1" t="s">
+      <c r="AC1" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="AD1" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="AE1" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="AF1" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="AG1" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="AD1" s="6" t="s">
+      <c r="AH1" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="AE1" s="6" t="s">
+      <c r="AI1" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="AF1" s="6" t="s">
+      <c r="AJ1" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="AG1" s="6" t="s">
+      <c r="AK1" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="AH1" s="4" t="s">
+      <c r="AL1" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="AI1" s="4" t="s">
+      <c r="AM1" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="AJ1" s="4" t="s">
+      <c r="AN1" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="AK1" s="4" t="s">
+      <c r="AO1" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="AL1" s="4" t="s">
+      <c r="AP1" s="3" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A2" s="2">
+    <row r="2" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="A2" s="10">
         <v>42856</v>
       </c>
-      <c r="B2" s="3">
+      <c r="B2" s="11">
         <v>229</v>
       </c>
-      <c r="D2" s="3">
+      <c r="D2" s="11">
         <v>309</v>
       </c>
-      <c r="E2" s="3">
+      <c r="E2" s="11">
         <v>67</v>
       </c>
-      <c r="F2" s="3">
+      <c r="F2" s="11">
         <v>3064</v>
       </c>
-      <c r="G2" s="3">
+      <c r="G2" s="11">
         <v>3</v>
       </c>
-      <c r="H2" s="3">
+      <c r="H2" s="11">
         <v>192</v>
       </c>
-      <c r="I2" s="3">
+      <c r="I2" s="11">
         <v>216</v>
       </c>
-      <c r="J2" s="3">
+      <c r="J2" s="11">
         <v>657</v>
       </c>
-      <c r="K2" s="3">
+      <c r="K2" s="11">
         <v>130</v>
       </c>
-      <c r="L2" s="3">
+      <c r="L2" s="11">
         <v>1</v>
       </c>
-      <c r="M2" s="3">
+      <c r="M2" s="11">
         <v>224</v>
       </c>
-      <c r="N2" s="3">
+      <c r="N2" s="11">
         <v>10</v>
       </c>
-      <c r="O2" s="3">
+      <c r="O2" s="11">
         <v>0</v>
       </c>
-      <c r="P2" s="3">
+      <c r="P2" s="11">
         <v>10</v>
       </c>
-      <c r="Q2" s="3">
+      <c r="Q2" s="11">
         <v>84</v>
       </c>
-      <c r="R2" s="3">
+      <c r="R2" s="11">
         <v>15</v>
       </c>
-      <c r="S2" s="3">
+      <c r="S2" s="11">
         <v>2</v>
       </c>
-      <c r="AD2" s="7"/>
-      <c r="AE2" s="7"/>
-      <c r="AF2" s="7"/>
-      <c r="AG2" s="7"/>
+      <c r="AD2" s="11"/>
+      <c r="AE2" s="11"/>
+      <c r="AF2" s="11"/>
+      <c r="AG2" s="11"/>
+      <c r="AH2" s="8"/>
+      <c r="AI2" s="8"/>
+      <c r="AJ2" s="8"/>
+      <c r="AK2" s="8"/>
+      <c r="AM2" s="4"/>
+      <c r="AN2" s="4"/>
+      <c r="AO2" s="4"/>
+      <c r="AP2" s="4"/>
     </row>
-    <row r="3" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A3" s="2">
+    <row r="3" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="A3" s="10">
         <v>42858</v>
       </c>
-      <c r="B3" s="3">
+      <c r="B3" s="11">
         <v>229</v>
       </c>
-      <c r="D3" s="3">
+      <c r="D3" s="11">
         <v>309</v>
       </c>
-      <c r="E3" s="3">
+      <c r="E3" s="11">
         <v>67</v>
       </c>
-      <c r="F3" s="3">
+      <c r="F3" s="11">
         <v>3554</v>
       </c>
-      <c r="G3" s="3">
+      <c r="G3" s="11">
         <v>3</v>
       </c>
-      <c r="H3" s="3">
+      <c r="H3" s="11">
         <v>192</v>
       </c>
-      <c r="I3" s="3">
+      <c r="I3" s="11">
         <v>216</v>
       </c>
-      <c r="J3" s="3">
+      <c r="J3" s="11">
         <v>657</v>
       </c>
-      <c r="K3" s="3">
+      <c r="K3" s="11">
         <v>130</v>
       </c>
-      <c r="L3" s="3">
+      <c r="L3" s="11">
         <v>1</v>
       </c>
-      <c r="M3" s="3">
+      <c r="M3" s="11">
         <v>224</v>
       </c>
-      <c r="N3" s="3">
+      <c r="N3" s="11">
         <v>10</v>
       </c>
-      <c r="O3" s="3">
+      <c r="O3" s="11">
         <v>0</v>
       </c>
-      <c r="P3" s="3">
+      <c r="P3" s="11">
         <v>10</v>
       </c>
-      <c r="Q3" s="3">
+      <c r="Q3" s="11">
         <v>83</v>
       </c>
-      <c r="R3" s="3">
+      <c r="R3" s="11">
         <v>15</v>
       </c>
-      <c r="S3" s="3">
+      <c r="S3" s="11">
         <v>2</v>
       </c>
-      <c r="AD3" s="7"/>
-      <c r="AE3" s="7"/>
-      <c r="AF3" s="7"/>
-      <c r="AG3" s="7"/>
+      <c r="AD3" s="11"/>
+      <c r="AE3" s="11"/>
+      <c r="AF3" s="11"/>
+      <c r="AG3" s="11"/>
+      <c r="AH3" s="8"/>
+      <c r="AI3" s="8"/>
+      <c r="AJ3" s="8"/>
+      <c r="AK3" s="8"/>
+      <c r="AM3" s="4"/>
+      <c r="AN3" s="4"/>
+      <c r="AO3" s="4"/>
+      <c r="AP3" s="4"/>
     </row>
-    <row r="4" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A4" s="2">
+    <row r="4" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="A4" s="10">
         <v>42859</v>
       </c>
-      <c r="B4" s="3">
+      <c r="B4" s="11">
         <v>229</v>
       </c>
-      <c r="D4" s="3">
+      <c r="D4" s="11">
         <v>309</v>
       </c>
-      <c r="E4" s="3">
+      <c r="E4" s="11">
         <v>67</v>
       </c>
-      <c r="F4" s="3">
+      <c r="F4" s="11">
         <v>3554</v>
       </c>
-      <c r="G4" s="3">
+      <c r="G4" s="11">
         <v>3</v>
       </c>
-      <c r="H4" s="3">
+      <c r="H4" s="11">
         <v>192</v>
       </c>
-      <c r="I4" s="3">
+      <c r="I4" s="11">
         <v>216</v>
       </c>
-      <c r="J4" s="3">
+      <c r="J4" s="11">
         <v>657</v>
       </c>
-      <c r="K4" s="3">
+      <c r="K4" s="11">
         <v>130</v>
       </c>
-      <c r="L4" s="3">
+      <c r="L4" s="11">
         <v>1</v>
       </c>
-      <c r="M4" s="3">
+      <c r="M4" s="11">
         <v>224</v>
       </c>
-      <c r="N4" s="3">
+      <c r="N4" s="11">
         <v>10</v>
       </c>
-      <c r="O4" s="3">
+      <c r="O4" s="11">
         <v>0</v>
       </c>
-      <c r="P4" s="3">
+      <c r="P4" s="11">
         <v>10</v>
       </c>
-      <c r="Q4" s="3">
+      <c r="Q4" s="11">
         <v>83</v>
       </c>
-      <c r="R4" s="3">
+      <c r="R4" s="11">
         <v>15</v>
       </c>
-      <c r="S4" s="3">
+      <c r="S4" s="11">
         <v>2</v>
       </c>
-      <c r="AD4" s="7"/>
-      <c r="AE4" s="7"/>
-      <c r="AF4" s="7"/>
-      <c r="AG4" s="7"/>
+      <c r="AD4" s="11"/>
+      <c r="AE4" s="11"/>
+      <c r="AF4" s="11"/>
+      <c r="AG4" s="11"/>
+      <c r="AH4" s="8"/>
+      <c r="AI4" s="8"/>
+      <c r="AJ4" s="8"/>
+      <c r="AK4" s="8"/>
+      <c r="AM4" s="4"/>
+      <c r="AN4" s="4"/>
+      <c r="AO4" s="4"/>
+      <c r="AP4" s="4"/>
     </row>
-    <row r="5" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A5" s="2">
+    <row r="5" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="A5" s="10">
         <v>42860</v>
       </c>
-      <c r="B5" s="3">
+      <c r="B5" s="11">
         <v>229</v>
       </c>
-      <c r="D5" s="3">
+      <c r="D5" s="11">
         <v>309</v>
       </c>
-      <c r="E5" s="3">
+      <c r="E5" s="11">
         <v>67</v>
       </c>
-      <c r="F5" s="3">
+      <c r="F5" s="11">
         <v>3555</v>
       </c>
-      <c r="G5" s="3">
+      <c r="G5" s="11">
         <v>3</v>
       </c>
-      <c r="H5" s="3">
+      <c r="H5" s="11">
         <v>202</v>
       </c>
-      <c r="I5" s="3">
+      <c r="I5" s="11">
         <v>216</v>
       </c>
-      <c r="J5" s="3">
+      <c r="J5" s="11">
         <v>657</v>
       </c>
-      <c r="K5" s="3">
+      <c r="K5" s="11">
         <v>130</v>
       </c>
-      <c r="L5" s="3">
+      <c r="L5" s="11">
         <v>1</v>
       </c>
-      <c r="M5" s="3">
+      <c r="M5" s="11">
         <v>225</v>
       </c>
-      <c r="N5" s="3">
+      <c r="N5" s="11">
         <v>10</v>
       </c>
-      <c r="O5" s="3">
+      <c r="O5" s="11">
         <v>0</v>
       </c>
-      <c r="P5" s="3">
+      <c r="P5" s="11">
         <v>10</v>
       </c>
-      <c r="Q5" s="3">
+      <c r="Q5" s="11">
         <v>83</v>
       </c>
-      <c r="R5" s="3">
+      <c r="R5" s="11">
         <v>15</v>
       </c>
-      <c r="S5" s="3">
+      <c r="S5" s="11">
         <v>1</v>
       </c>
-      <c r="AD5" s="7"/>
-      <c r="AE5" s="7"/>
-      <c r="AF5" s="7"/>
-      <c r="AG5" s="7"/>
+      <c r="AD5" s="11"/>
+      <c r="AE5" s="11"/>
+      <c r="AF5" s="11"/>
+      <c r="AG5" s="11"/>
+      <c r="AH5" s="8"/>
+      <c r="AI5" s="8"/>
+      <c r="AJ5" s="8"/>
+      <c r="AK5" s="8"/>
+      <c r="AM5" s="4"/>
+      <c r="AN5" s="4"/>
+      <c r="AO5" s="4"/>
+      <c r="AP5" s="4"/>
     </row>
-    <row r="6" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A6" s="2">
+    <row r="6" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="A6" s="10">
         <v>42861</v>
       </c>
-      <c r="B6" s="3">
+      <c r="B6" s="11">
         <v>229</v>
       </c>
-      <c r="D6" s="3">
+      <c r="D6" s="11">
         <v>309</v>
       </c>
-      <c r="E6" s="3">
+      <c r="E6" s="11">
         <v>67</v>
       </c>
-      <c r="F6" s="3">
+      <c r="F6" s="11">
         <v>3555</v>
       </c>
-      <c r="G6" s="3">
+      <c r="G6" s="11">
         <v>3</v>
       </c>
-      <c r="H6" s="3">
+      <c r="H6" s="11">
         <v>202</v>
       </c>
-      <c r="I6" s="3">
+      <c r="I6" s="11">
         <v>216</v>
       </c>
-      <c r="J6" s="3">
+      <c r="J6" s="11">
         <v>657</v>
       </c>
-      <c r="K6" s="3">
+      <c r="K6" s="11">
         <v>130</v>
       </c>
-      <c r="L6" s="3">
+      <c r="L6" s="11">
         <v>1</v>
       </c>
-      <c r="M6" s="3">
+      <c r="M6" s="11">
         <v>225</v>
       </c>
-      <c r="N6" s="3">
+      <c r="N6" s="11">
         <v>10</v>
       </c>
-      <c r="O6" s="3">
+      <c r="O6" s="11">
         <v>0</v>
       </c>
-      <c r="P6" s="3">
+      <c r="P6" s="11">
         <v>10</v>
       </c>
-      <c r="Q6" s="3">
+      <c r="Q6" s="11">
         <v>83</v>
       </c>
-      <c r="R6" s="3">
+      <c r="R6" s="11">
         <v>15</v>
       </c>
-      <c r="S6" s="3">
+      <c r="S6" s="11">
         <v>1</v>
       </c>
-      <c r="T6" s="3">
+      <c r="T6" s="11">
         <v>7</v>
       </c>
-      <c r="U6" s="3">
+      <c r="U6" s="11">
         <v>7</v>
       </c>
-      <c r="V6" s="3">
+      <c r="V6" s="11">
         <v>88</v>
       </c>
-      <c r="W6" s="3">
+      <c r="W6" s="11">
         <v>19</v>
       </c>
-      <c r="X6" s="3">
+      <c r="X6" s="11">
         <v>42</v>
       </c>
-      <c r="AD6" s="7"/>
-      <c r="AE6" s="7"/>
-      <c r="AF6" s="7"/>
-      <c r="AG6" s="7"/>
+      <c r="AD6" s="11"/>
+      <c r="AE6" s="11"/>
+      <c r="AF6" s="11"/>
+      <c r="AG6" s="11"/>
+      <c r="AH6" s="8"/>
+      <c r="AI6" s="8"/>
+      <c r="AJ6" s="8"/>
+      <c r="AK6" s="8"/>
+      <c r="AM6" s="4"/>
+      <c r="AN6" s="4"/>
+      <c r="AO6" s="4"/>
+      <c r="AP6" s="4"/>
     </row>
-    <row r="7" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A7" s="2">
+    <row r="7" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="A7" s="10">
         <v>42864</v>
       </c>
-      <c r="B7" s="3">
+      <c r="B7" s="11">
         <v>229</v>
       </c>
-      <c r="C7" s="3">
+      <c r="C7" s="11">
         <v>5</v>
       </c>
-      <c r="D7" s="3">
+      <c r="D7" s="11">
         <v>309</v>
       </c>
-      <c r="E7" s="3">
+      <c r="E7" s="11">
         <v>67</v>
       </c>
-      <c r="F7" s="3">
+      <c r="F7" s="11">
         <v>3555</v>
       </c>
-      <c r="G7" s="3">
+      <c r="G7" s="11">
         <v>3</v>
       </c>
-      <c r="H7" s="3">
+      <c r="H7" s="11">
         <v>202</v>
       </c>
-      <c r="I7" s="3">
+      <c r="I7" s="11">
         <v>216</v>
       </c>
-      <c r="J7" s="3">
+      <c r="J7" s="11">
         <v>657</v>
       </c>
-      <c r="K7" s="3">
+      <c r="K7" s="11">
         <v>130</v>
       </c>
-      <c r="L7" s="3">
+      <c r="L7" s="11">
         <v>1</v>
       </c>
-      <c r="M7" s="3">
+      <c r="M7" s="11">
         <v>225</v>
       </c>
-      <c r="N7" s="3">
+      <c r="N7" s="11">
         <v>10</v>
       </c>
-      <c r="O7" s="3">
+      <c r="O7" s="11">
         <v>0</v>
       </c>
-      <c r="P7" s="3">
+      <c r="P7" s="11">
         <v>10</v>
       </c>
-      <c r="Q7" s="3">
+      <c r="Q7" s="11">
         <v>83</v>
       </c>
-      <c r="R7" s="3">
+      <c r="R7" s="11">
         <v>15</v>
       </c>
-      <c r="S7" s="3">
+      <c r="S7" s="11">
         <v>1</v>
       </c>
-      <c r="T7" s="3">
+      <c r="T7" s="11">
         <v>7</v>
       </c>
-      <c r="U7" s="3">
+      <c r="U7" s="11">
         <v>7</v>
       </c>
-      <c r="V7" s="3">
+      <c r="V7" s="11">
         <v>88</v>
       </c>
-      <c r="W7" s="3">
+      <c r="W7" s="11">
         <v>19</v>
       </c>
-      <c r="X7" s="3">
+      <c r="X7" s="11">
         <v>42</v>
       </c>
-      <c r="Y7" s="3">
+      <c r="Y7" s="11">
         <v>45</v>
       </c>
-      <c r="Z7" s="3">
+      <c r="Z7" s="11">
         <v>240</v>
       </c>
-      <c r="AA7" s="3">
+      <c r="AA7" s="11">
         <v>130</v>
       </c>
-      <c r="AB7" s="3">
+      <c r="AB7" s="11">
         <v>0</v>
       </c>
-      <c r="AC7" s="3">
+      <c r="AD7" s="11"/>
+      <c r="AE7" s="11"/>
+      <c r="AF7" s="11"/>
+      <c r="AG7" s="11">
         <v>229</v>
       </c>
-      <c r="AD7" s="8">
+      <c r="AH7" s="6">
         <v>3</v>
       </c>
-      <c r="AE7" s="8">
+      <c r="AI7" s="6">
         <v>25</v>
       </c>
-      <c r="AF7" s="8">
+      <c r="AJ7" s="6">
         <v>77</v>
       </c>
-      <c r="AG7" s="8">
+      <c r="AK7" s="6">
         <v>353</v>
       </c>
-      <c r="AH7" s="5">
+      <c r="AL7" s="4">
         <v>1</v>
       </c>
-      <c r="AI7" s="5">
+      <c r="AM7" s="4">
         <v>0.6</v>
       </c>
-      <c r="AJ7" s="5">
+      <c r="AN7" s="4">
         <v>0.37313429999999997</v>
       </c>
-      <c r="AK7" s="5">
+      <c r="AO7" s="4">
         <v>0.24919089999999999</v>
       </c>
-      <c r="AL7" s="5">
+      <c r="AP7" s="4">
         <v>9.9296759999999998E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A8" s="2">
+    <row r="8" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="A8" s="10">
         <v>42865</v>
       </c>
-      <c r="B8" s="3">
+      <c r="B8" s="11">
         <v>229</v>
       </c>
-      <c r="C8" s="3">
+      <c r="C8" s="11">
         <v>5</v>
       </c>
-      <c r="D8" s="3">
+      <c r="D8" s="11">
         <v>309</v>
       </c>
-      <c r="E8" s="3">
+      <c r="E8" s="11">
         <v>67</v>
       </c>
-      <c r="F8" s="3">
+      <c r="F8" s="11">
         <v>3555</v>
       </c>
-      <c r="G8" s="3">
+      <c r="G8" s="11">
         <v>3</v>
       </c>
-      <c r="H8" s="3">
+      <c r="H8" s="11">
         <v>202</v>
       </c>
-      <c r="I8" s="3">
+      <c r="I8" s="11">
         <v>216</v>
       </c>
-      <c r="J8" s="3">
+      <c r="J8" s="11">
         <v>657</v>
       </c>
-      <c r="K8" s="3">
+      <c r="K8" s="11">
         <v>130</v>
       </c>
-      <c r="L8" s="3">
+      <c r="L8" s="11">
         <v>1</v>
       </c>
-      <c r="M8" s="3">
+      <c r="M8" s="11">
         <v>225</v>
       </c>
-      <c r="N8" s="3">
+      <c r="N8" s="11">
         <v>10</v>
       </c>
-      <c r="O8" s="3">
+      <c r="O8" s="11">
         <v>0</v>
       </c>
-      <c r="P8" s="3">
+      <c r="P8" s="11">
         <v>10</v>
       </c>
-      <c r="Q8" s="3">
+      <c r="Q8" s="11">
         <v>83</v>
       </c>
-      <c r="R8" s="3">
+      <c r="R8" s="11">
         <v>15</v>
       </c>
-      <c r="S8" s="3">
+      <c r="S8" s="11">
         <v>1</v>
       </c>
-      <c r="T8" s="3">
+      <c r="T8" s="11">
         <v>7</v>
       </c>
-      <c r="U8" s="3">
+      <c r="U8" s="11">
         <v>7</v>
       </c>
-      <c r="V8" s="3">
+      <c r="V8" s="11">
         <v>83</v>
       </c>
-      <c r="W8" s="3">
+      <c r="W8" s="11">
         <v>19</v>
       </c>
-      <c r="X8" s="3">
+      <c r="X8" s="11">
         <v>15</v>
       </c>
-      <c r="Y8" s="3">
+      <c r="Y8" s="11">
         <v>45</v>
       </c>
-      <c r="Z8" s="3">
+      <c r="Z8" s="11">
         <v>240</v>
       </c>
-      <c r="AA8" s="3">
+      <c r="AA8" s="11">
         <v>130</v>
       </c>
-      <c r="AB8" s="3">
+      <c r="AB8" s="11">
         <v>0</v>
       </c>
-      <c r="AC8" s="3">
+      <c r="AD8" s="11"/>
+      <c r="AE8" s="11"/>
+      <c r="AF8" s="11"/>
+      <c r="AG8" s="11">
         <v>229</v>
       </c>
-      <c r="AD8" s="8">
+      <c r="AH8" s="6">
         <v>5</v>
       </c>
-      <c r="AE8" s="8">
+      <c r="AI8" s="6">
         <v>30</v>
       </c>
-      <c r="AF8" s="8">
+      <c r="AJ8" s="6">
         <v>85</v>
       </c>
-      <c r="AG8" s="8">
+      <c r="AK8" s="6">
         <v>503</v>
       </c>
-      <c r="AH8" s="5">
+      <c r="AL8" s="4">
         <v>1</v>
       </c>
-      <c r="AI8" s="5">
+      <c r="AM8" s="4">
         <v>1</v>
       </c>
-      <c r="AJ8" s="5">
+      <c r="AN8" s="4">
         <v>0.44776120000000003</v>
       </c>
-      <c r="AK8" s="5">
+      <c r="AO8" s="4">
         <v>0.27508090000000002</v>
       </c>
-      <c r="AL8" s="5">
+      <c r="AP8" s="4">
         <v>0.1414909</v>
       </c>
     </row>
-    <row r="9" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A9" s="2">
+    <row r="9" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="A9" s="10">
         <v>42867</v>
       </c>
-      <c r="B9" s="3">
+      <c r="B9" s="11">
         <v>229</v>
       </c>
-      <c r="C9" s="3">
+      <c r="C9" s="11">
         <v>5</v>
       </c>
-      <c r="D9" s="3">
+      <c r="D9" s="11">
         <v>309</v>
       </c>
-      <c r="E9" s="3">
+      <c r="E9" s="11">
         <v>67</v>
       </c>
-      <c r="F9" s="3">
+      <c r="F9" s="11">
         <v>3555</v>
       </c>
-      <c r="G9" s="3">
+      <c r="G9" s="11">
         <v>3</v>
       </c>
-      <c r="H9" s="3">
+      <c r="H9" s="11">
         <v>202</v>
       </c>
-      <c r="I9" s="3">
+      <c r="I9" s="11">
         <v>216</v>
       </c>
-      <c r="J9" s="3">
+      <c r="J9" s="11">
         <v>657</v>
       </c>
-      <c r="K9" s="3">
+      <c r="K9" s="11">
         <v>130</v>
       </c>
-      <c r="L9" s="3">
+      <c r="L9" s="11">
         <v>1</v>
       </c>
-      <c r="M9" s="3">
+      <c r="M9" s="11">
         <v>225</v>
       </c>
-      <c r="N9" s="3">
+      <c r="N9" s="11">
         <v>10</v>
       </c>
-      <c r="O9" s="3">
+      <c r="O9" s="11">
         <v>0</v>
       </c>
-      <c r="P9" s="3">
+      <c r="P9" s="11">
         <v>10</v>
       </c>
-      <c r="Q9" s="3">
+      <c r="Q9" s="11">
         <v>83</v>
       </c>
-      <c r="R9" s="3">
+      <c r="R9" s="11">
         <v>15</v>
       </c>
-      <c r="S9" s="3">
+      <c r="S9" s="11">
         <v>1</v>
       </c>
-      <c r="T9" s="3">
+      <c r="T9" s="11">
         <v>7</v>
       </c>
-      <c r="U9" s="3">
+      <c r="U9" s="11">
         <v>7</v>
       </c>
-      <c r="V9" s="3">
+      <c r="V9" s="11">
         <v>83</v>
       </c>
-      <c r="W9" s="3">
+      <c r="W9" s="11">
         <v>19</v>
       </c>
-      <c r="X9" s="3">
+      <c r="X9" s="11">
         <v>15</v>
       </c>
-      <c r="Y9" s="3">
+      <c r="Y9" s="11">
         <v>45</v>
       </c>
-      <c r="Z9" s="3">
+      <c r="Z9" s="11">
         <v>240</v>
       </c>
-      <c r="AA9" s="3">
+      <c r="AA9" s="11">
         <v>130</v>
       </c>
-      <c r="AB9" s="3">
+      <c r="AB9" s="11">
         <v>0</v>
       </c>
-      <c r="AC9" s="3">
+      <c r="AC9" s="11">
+        <v>237</v>
+      </c>
+      <c r="AD9" s="6">
+        <v>137</v>
+      </c>
+      <c r="AE9" s="6">
+        <v>3</v>
+      </c>
+      <c r="AF9" s="6">
+        <v>3</v>
+      </c>
+      <c r="AG9" s="6">
         <v>229</v>
       </c>
-      <c r="AD9" s="8">
+      <c r="AH9" s="6">
         <v>5</v>
       </c>
-      <c r="AE9" s="8">
-        <v>30</v>
-      </c>
-      <c r="AF9" s="8">
-        <v>85</v>
-      </c>
-      <c r="AG9" s="8">
-        <v>503</v>
-      </c>
-      <c r="AH9" s="5">
+      <c r="AI9" s="6">
+        <v>38</v>
+      </c>
+      <c r="AJ9" s="6">
+        <v>102</v>
+      </c>
+      <c r="AK9" s="6">
+        <v>1170</v>
+      </c>
+      <c r="AL9" s="4">
         <v>1</v>
       </c>
-      <c r="AI9" s="5">
+      <c r="AM9" s="5">
         <v>1</v>
       </c>
-      <c r="AJ9" s="5">
-        <v>0.44776120000000003</v>
-      </c>
-      <c r="AK9" s="5">
-        <v>0.27508090000000002</v>
-      </c>
-      <c r="AL9" s="5">
-        <v>0.1414909</v>
+      <c r="AN9" s="5">
+        <v>0.56716420000000001</v>
+      </c>
+      <c r="AO9" s="5">
+        <v>0.33009709999999998</v>
+      </c>
+      <c r="AP9" s="5">
+        <v>0.32911390000000001</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
SNAPSHOT_v11.1d_2017-06-05. Created sample app.
</commit_message>
<xml_diff>
--- a/referenceDocsMetrics.xlsx
+++ b/referenceDocsMetrics.xlsx
@@ -148,7 +148,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -178,8 +178,22 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -189,6 +203,16 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
       </patternFill>
     </fill>
   </fills>
@@ -201,12 +225,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -238,9 +264,23 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="3" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="4" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="3" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="5">
     <cellStyle name="Accent1" xfId="1" builtinId="29"/>
+    <cellStyle name="Bad" xfId="4" builtinId="27"/>
+    <cellStyle name="Good" xfId="3" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="2" builtinId="5"/>
   </cellStyles>
@@ -293,10 +333,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$A$2:$A$13</c:f>
+              <c:f>Sheet1!$A$2:$A$19</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="12"/>
+                <c:ptCount val="18"/>
                 <c:pt idx="0">
                   <c:v>42864</c:v>
                 </c:pt>
@@ -332,16 +372,34 @@
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>42878</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>42880</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>42884</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>42885</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>42887</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>42888</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>42891</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$G$2:$G$13</c:f>
+              <c:f>Sheet1!$G$2:$G$19</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="12"/>
+                <c:ptCount val="18"/>
                 <c:pt idx="0">
                   <c:v>3</c:v>
                 </c:pt>
@@ -377,6 +435,24 @@
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -402,10 +478,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$A$2:$A$13</c:f>
+              <c:f>Sheet1!$A$2:$A$19</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="12"/>
+                <c:ptCount val="18"/>
                 <c:pt idx="0">
                   <c:v>42864</c:v>
                 </c:pt>
@@ -441,16 +517,34 @@
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>42878</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>42880</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>42884</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>42885</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>42887</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>42888</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>42891</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$H$2:$H$13</c:f>
+              <c:f>Sheet1!$H$2:$H$19</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="12"/>
+                <c:ptCount val="18"/>
                 <c:pt idx="0">
                   <c:v>202</c:v>
                 </c:pt>
@@ -485,6 +579,24 @@
                   <c:v>66</c:v>
                 </c:pt>
                 <c:pt idx="11">
+                  <c:v>62</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>62</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>62</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>62</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>62</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>62</c:v>
+                </c:pt>
+                <c:pt idx="17">
                   <c:v>62</c:v>
                 </c:pt>
               </c:numCache>
@@ -511,10 +623,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$A$2:$A$13</c:f>
+              <c:f>Sheet1!$A$2:$A$19</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="12"/>
+                <c:ptCount val="18"/>
                 <c:pt idx="0">
                   <c:v>42864</c:v>
                 </c:pt>
@@ -550,16 +662,34 @@
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>42878</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>42880</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>42884</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>42885</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>42887</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>42888</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>42891</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$I$2:$I$13</c:f>
+              <c:f>Sheet1!$I$2:$I$19</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="12"/>
+                <c:ptCount val="18"/>
                 <c:pt idx="0">
                   <c:v>216</c:v>
                 </c:pt>
@@ -594,6 +724,24 @@
                   <c:v>216</c:v>
                 </c:pt>
                 <c:pt idx="11">
+                  <c:v>216</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>216</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>216</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>216</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>216</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>216</c:v>
+                </c:pt>
+                <c:pt idx="17">
                   <c:v>216</c:v>
                 </c:pt>
               </c:numCache>
@@ -620,10 +768,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$A$2:$A$13</c:f>
+              <c:f>Sheet1!$A$2:$A$19</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="12"/>
+                <c:ptCount val="18"/>
                 <c:pt idx="0">
                   <c:v>42864</c:v>
                 </c:pt>
@@ -659,16 +807,34 @@
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>42878</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>42880</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>42884</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>42885</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>42887</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>42888</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>42891</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$J$2:$J$13</c:f>
+              <c:f>Sheet1!$J$2:$J$19</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="12"/>
+                <c:ptCount val="18"/>
                 <c:pt idx="0">
                   <c:v>657</c:v>
                 </c:pt>
@@ -703,6 +869,24 @@
                   <c:v>657</c:v>
                 </c:pt>
                 <c:pt idx="11">
+                  <c:v>657</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>657</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>657</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>657</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>657</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>657</c:v>
+                </c:pt>
+                <c:pt idx="17">
                   <c:v>657</c:v>
                 </c:pt>
               </c:numCache>
@@ -729,10 +913,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$A$2:$A$13</c:f>
+              <c:f>Sheet1!$A$2:$A$19</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="12"/>
+                <c:ptCount val="18"/>
                 <c:pt idx="0">
                   <c:v>42864</c:v>
                 </c:pt>
@@ -768,16 +952,34 @@
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>42878</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>42880</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>42884</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>42885</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>42887</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>42888</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>42891</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$K$2:$K$13</c:f>
+              <c:f>Sheet1!$K$2:$K$19</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="12"/>
+                <c:ptCount val="18"/>
                 <c:pt idx="0">
                   <c:v>130</c:v>
                 </c:pt>
@@ -812,6 +1014,24 @@
                   <c:v>130</c:v>
                 </c:pt>
                 <c:pt idx="11">
+                  <c:v>130</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>130</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>130</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>130</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>130</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>130</c:v>
+                </c:pt>
+                <c:pt idx="17">
                   <c:v>130</c:v>
                 </c:pt>
               </c:numCache>
@@ -829,11 +1049,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="92931200"/>
-        <c:axId val="92932736"/>
+        <c:axId val="67624960"/>
+        <c:axId val="67626496"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="92931200"/>
+        <c:axId val="67624960"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -843,14 +1063,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="92932736"/>
+        <c:crossAx val="67626496"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="92932736"/>
+        <c:axId val="67626496"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -861,7 +1081,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="92931200"/>
+        <c:crossAx val="67624960"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -904,8 +1124,8 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="3.757892519400368E-2"/>
-          <c:y val="1.7058056422192509E-2"/>
+          <c:x val="6.5272345295232889E-2"/>
+          <c:y val="4.2215289126595022E-2"/>
           <c:w val="0.67996879999544524"/>
           <c:h val="0.82352630449495701"/>
         </c:manualLayout>
@@ -932,10 +1152,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$A$2:$A$13</c:f>
+              <c:f>Sheet1!$A$2:$A$19</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="12"/>
+                <c:ptCount val="18"/>
                 <c:pt idx="0">
                   <c:v>42864</c:v>
                 </c:pt>
@@ -971,16 +1191,34 @@
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>42878</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>42880</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>42884</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>42885</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>42887</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>42888</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>42891</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$AL$2:$AL$13</c:f>
+              <c:f>Sheet1!$AL$2:$AL$19</c:f>
               <c:numCache>
                 <c:formatCode>0%</c:formatCode>
-                <c:ptCount val="12"/>
+                <c:ptCount val="18"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -1015,6 +1253,24 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="11">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="17">
                   <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
@@ -1041,10 +1297,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$A$2:$A$13</c:f>
+              <c:f>Sheet1!$A$2:$A$19</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="12"/>
+                <c:ptCount val="18"/>
                 <c:pt idx="0">
                   <c:v>42864</c:v>
                 </c:pt>
@@ -1080,16 +1336,34 @@
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>42878</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>42880</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>42884</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>42885</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>42887</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>42888</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>42891</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$AM$2:$AM$13</c:f>
+              <c:f>Sheet1!$AM$2:$AM$19</c:f>
               <c:numCache>
                 <c:formatCode>0%</c:formatCode>
-                <c:ptCount val="12"/>
+                <c:ptCount val="18"/>
                 <c:pt idx="0">
                   <c:v>0.6</c:v>
                 </c:pt>
@@ -1124,6 +1398,24 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="11">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="17">
                   <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
@@ -1150,10 +1442,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$A$2:$A$13</c:f>
+              <c:f>Sheet1!$A$2:$A$19</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="12"/>
+                <c:ptCount val="18"/>
                 <c:pt idx="0">
                   <c:v>42864</c:v>
                 </c:pt>
@@ -1189,16 +1481,34 @@
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>42878</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>42880</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>42884</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>42885</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>42887</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>42888</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>42891</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$AN$2:$AN$13</c:f>
+              <c:f>Sheet1!$AN$2:$AN$19</c:f>
               <c:numCache>
                 <c:formatCode>0%</c:formatCode>
-                <c:ptCount val="12"/>
+                <c:ptCount val="18"/>
                 <c:pt idx="0">
                   <c:v>0.37313429999999997</c:v>
                 </c:pt>
@@ -1233,6 +1543,24 @@
                   <c:v>0.98507460000000002</c:v>
                 </c:pt>
                 <c:pt idx="11">
+                  <c:v>0.98507460000000002</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.98507460000000002</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.98507460000000002</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.98507460000000002</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.98507460000000002</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.98507460000000002</c:v>
+                </c:pt>
+                <c:pt idx="17">
                   <c:v>0.98507460000000002</c:v>
                 </c:pt>
               </c:numCache>
@@ -1259,10 +1587,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$A$2:$A$13</c:f>
+              <c:f>Sheet1!$A$2:$A$19</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="12"/>
+                <c:ptCount val="18"/>
                 <c:pt idx="0">
                   <c:v>42864</c:v>
                 </c:pt>
@@ -1298,16 +1626,34 @@
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>42878</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>42880</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>42884</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>42885</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>42887</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>42888</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>42891</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$AO$2:$AO$13</c:f>
+              <c:f>Sheet1!$AO$2:$AO$19</c:f>
               <c:numCache>
                 <c:formatCode>0%</c:formatCode>
-                <c:ptCount val="12"/>
+                <c:ptCount val="18"/>
                 <c:pt idx="0">
                   <c:v>0.24919089999999999</c:v>
                 </c:pt>
@@ -1343,6 +1689,24 @@
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>0.37540449999999997</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.3786408</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.3786408</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.3786408</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.3786408</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.3786408</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.3786408</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1368,10 +1732,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$A$2:$A$13</c:f>
+              <c:f>Sheet1!$A$2:$A$19</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="12"/>
+                <c:ptCount val="18"/>
                 <c:pt idx="0">
                   <c:v>42864</c:v>
                 </c:pt>
@@ -1407,16 +1771,34 @@
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>42878</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>42880</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>42884</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>42885</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>42887</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>42888</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>42891</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$AP$2:$AP$13</c:f>
+              <c:f>Sheet1!$AP$2:$AP$19</c:f>
               <c:numCache>
                 <c:formatCode>0%</c:formatCode>
-                <c:ptCount val="12"/>
+                <c:ptCount val="18"/>
                 <c:pt idx="0">
                   <c:v>9.9296759999999998E-2</c:v>
                 </c:pt>
@@ -1452,6 +1834,24 @@
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>0.70890699999999995</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.707982</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.70806409999999997</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.70806409999999997</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.70806409999999997</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.70806409999999997</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.70946900000000002</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1468,11 +1868,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="92972544"/>
-        <c:axId val="92974080"/>
+        <c:axId val="73884032"/>
+        <c:axId val="73885568"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="92972544"/>
+        <c:axId val="73884032"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1482,14 +1882,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="92974080"/>
+        <c:crossAx val="73885568"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="92974080"/>
+        <c:axId val="73885568"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1500,7 +1900,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="92972544"/>
+        <c:crossAx val="73884032"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1527,15 +1927,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>314325</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>104774</xdr:rowOff>
+      <xdr:colOff>257175</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>9524</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
-      <xdr:colOff>152400</xdr:colOff>
-      <xdr:row>38</xdr:row>
-      <xdr:rowOff>76199</xdr:rowOff>
+      <xdr:colOff>95250</xdr:colOff>
+      <xdr:row>53</xdr:row>
+      <xdr:rowOff>171449</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1557,15 +1957,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>16</xdr:col>
-      <xdr:colOff>333375</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>104775</xdr:rowOff>
+      <xdr:colOff>466725</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>26</xdr:col>
-      <xdr:colOff>466725</xdr:colOff>
-      <xdr:row>38</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
+      <xdr:colOff>600075</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1876,10 +2276,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AP13"/>
+  <dimension ref="A1:AQ19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14:XFD14"/>
+    <sheetView tabSelected="1" topLeftCell="X1" workbookViewId="0">
+      <selection activeCell="Q19" sqref="Q19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3564,6 +3964,775 @@
         <v>0.70890699999999995</v>
       </c>
     </row>
+    <row r="14" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="A14" s="9">
+        <v>42880</v>
+      </c>
+      <c r="B14" s="10">
+        <v>229</v>
+      </c>
+      <c r="C14" s="10">
+        <v>5</v>
+      </c>
+      <c r="D14" s="10">
+        <v>309</v>
+      </c>
+      <c r="E14" s="10">
+        <v>67</v>
+      </c>
+      <c r="F14" s="10">
+        <v>3558</v>
+      </c>
+      <c r="G14" s="10">
+        <v>3</v>
+      </c>
+      <c r="H14" s="10">
+        <v>62</v>
+      </c>
+      <c r="I14" s="10">
+        <v>216</v>
+      </c>
+      <c r="J14" s="10">
+        <v>657</v>
+      </c>
+      <c r="K14" s="10">
+        <v>130</v>
+      </c>
+      <c r="L14" s="10">
+        <v>1</v>
+      </c>
+      <c r="M14" s="10">
+        <v>225</v>
+      </c>
+      <c r="N14" s="10">
+        <v>10</v>
+      </c>
+      <c r="O14" s="10">
+        <v>0</v>
+      </c>
+      <c r="P14" s="10">
+        <v>10</v>
+      </c>
+      <c r="Q14" s="10">
+        <v>85</v>
+      </c>
+      <c r="R14" s="10">
+        <v>15</v>
+      </c>
+      <c r="S14" s="10">
+        <v>1</v>
+      </c>
+      <c r="T14" s="10">
+        <v>7</v>
+      </c>
+      <c r="U14" s="10">
+        <v>7</v>
+      </c>
+      <c r="V14" s="10">
+        <v>83</v>
+      </c>
+      <c r="W14" s="10">
+        <v>18</v>
+      </c>
+      <c r="X14" s="10">
+        <v>15</v>
+      </c>
+      <c r="Y14" s="10">
+        <v>45</v>
+      </c>
+      <c r="Z14" s="10">
+        <v>240</v>
+      </c>
+      <c r="AA14" s="10">
+        <v>130</v>
+      </c>
+      <c r="AB14" s="10">
+        <v>0</v>
+      </c>
+      <c r="AC14" s="10">
+        <v>237</v>
+      </c>
+      <c r="AD14" s="6">
+        <v>137</v>
+      </c>
+      <c r="AE14" s="6">
+        <v>3</v>
+      </c>
+      <c r="AF14" s="6">
+        <v>3</v>
+      </c>
+      <c r="AG14" s="6">
+        <v>229</v>
+      </c>
+      <c r="AH14" s="6">
+        <v>5</v>
+      </c>
+      <c r="AI14" s="6">
+        <v>66</v>
+      </c>
+      <c r="AJ14" s="6">
+        <v>117</v>
+      </c>
+      <c r="AK14" s="6">
+        <v>2519</v>
+      </c>
+      <c r="AL14" s="4">
+        <v>1</v>
+      </c>
+      <c r="AM14" s="5">
+        <v>1</v>
+      </c>
+      <c r="AN14" s="5">
+        <v>0.98507460000000002</v>
+      </c>
+      <c r="AO14" s="5">
+        <v>0.3786408</v>
+      </c>
+      <c r="AP14" s="5">
+        <v>0.707982</v>
+      </c>
+    </row>
+    <row r="15" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="A15" s="9">
+        <v>42884</v>
+      </c>
+      <c r="B15" s="10">
+        <v>229</v>
+      </c>
+      <c r="C15" s="10">
+        <v>5</v>
+      </c>
+      <c r="D15" s="10">
+        <v>309</v>
+      </c>
+      <c r="E15" s="10">
+        <v>67</v>
+      </c>
+      <c r="F15" s="10">
+        <v>3559</v>
+      </c>
+      <c r="G15" s="10">
+        <v>3</v>
+      </c>
+      <c r="H15" s="10">
+        <v>62</v>
+      </c>
+      <c r="I15" s="10">
+        <v>216</v>
+      </c>
+      <c r="J15" s="10">
+        <v>657</v>
+      </c>
+      <c r="K15" s="10">
+        <v>130</v>
+      </c>
+      <c r="L15" s="10">
+        <v>1</v>
+      </c>
+      <c r="M15" s="10">
+        <v>226</v>
+      </c>
+      <c r="N15" s="10">
+        <v>10</v>
+      </c>
+      <c r="O15" s="10">
+        <v>0</v>
+      </c>
+      <c r="P15" s="10">
+        <v>10</v>
+      </c>
+      <c r="Q15" s="10">
+        <v>85</v>
+      </c>
+      <c r="R15" s="10">
+        <v>15</v>
+      </c>
+      <c r="S15" s="10">
+        <v>1</v>
+      </c>
+      <c r="T15" s="10">
+        <v>7</v>
+      </c>
+      <c r="U15" s="10">
+        <v>7</v>
+      </c>
+      <c r="V15" s="10">
+        <v>83</v>
+      </c>
+      <c r="W15" s="10">
+        <v>18</v>
+      </c>
+      <c r="X15" s="10">
+        <v>15</v>
+      </c>
+      <c r="Y15" s="10">
+        <v>45</v>
+      </c>
+      <c r="Z15" s="10">
+        <v>240</v>
+      </c>
+      <c r="AA15" s="10">
+        <v>130</v>
+      </c>
+      <c r="AB15" s="10">
+        <v>0</v>
+      </c>
+      <c r="AC15" s="10">
+        <v>237</v>
+      </c>
+      <c r="AD15" s="6">
+        <v>137</v>
+      </c>
+      <c r="AE15" s="6">
+        <v>3</v>
+      </c>
+      <c r="AF15" s="6">
+        <v>3</v>
+      </c>
+      <c r="AG15" s="6">
+        <v>229</v>
+      </c>
+      <c r="AH15" s="6">
+        <v>5</v>
+      </c>
+      <c r="AI15" s="6">
+        <v>66</v>
+      </c>
+      <c r="AJ15" s="6">
+        <v>117</v>
+      </c>
+      <c r="AK15" s="6">
+        <v>2520</v>
+      </c>
+      <c r="AL15" s="4">
+        <v>1</v>
+      </c>
+      <c r="AM15" s="5">
+        <v>1</v>
+      </c>
+      <c r="AN15" s="5">
+        <v>0.98507460000000002</v>
+      </c>
+      <c r="AO15" s="5">
+        <v>0.3786408</v>
+      </c>
+      <c r="AP15" s="5">
+        <v>0.70806409999999997</v>
+      </c>
+    </row>
+    <row r="16" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="A16" s="9">
+        <v>42885</v>
+      </c>
+      <c r="B16" s="10">
+        <v>229</v>
+      </c>
+      <c r="C16" s="10">
+        <v>5</v>
+      </c>
+      <c r="D16" s="10">
+        <v>309</v>
+      </c>
+      <c r="E16" s="10">
+        <v>67</v>
+      </c>
+      <c r="F16" s="10">
+        <v>3559</v>
+      </c>
+      <c r="G16" s="10">
+        <v>3</v>
+      </c>
+      <c r="H16" s="10">
+        <v>62</v>
+      </c>
+      <c r="I16" s="10">
+        <v>216</v>
+      </c>
+      <c r="J16" s="10">
+        <v>657</v>
+      </c>
+      <c r="K16" s="10">
+        <v>130</v>
+      </c>
+      <c r="L16" s="10">
+        <v>1</v>
+      </c>
+      <c r="M16" s="10">
+        <v>226</v>
+      </c>
+      <c r="N16" s="10">
+        <v>10</v>
+      </c>
+      <c r="O16" s="10">
+        <v>0</v>
+      </c>
+      <c r="P16" s="10">
+        <v>10</v>
+      </c>
+      <c r="Q16" s="10">
+        <v>85</v>
+      </c>
+      <c r="R16" s="10">
+        <v>15</v>
+      </c>
+      <c r="S16" s="10">
+        <v>1</v>
+      </c>
+      <c r="T16" s="10">
+        <v>7</v>
+      </c>
+      <c r="U16" s="10">
+        <v>7</v>
+      </c>
+      <c r="V16" s="10">
+        <v>83</v>
+      </c>
+      <c r="W16" s="10">
+        <v>18</v>
+      </c>
+      <c r="X16" s="10">
+        <v>15</v>
+      </c>
+      <c r="Y16" s="10">
+        <v>45</v>
+      </c>
+      <c r="Z16" s="10">
+        <v>240</v>
+      </c>
+      <c r="AA16" s="10">
+        <v>130</v>
+      </c>
+      <c r="AB16" s="10">
+        <v>0</v>
+      </c>
+      <c r="AC16" s="10">
+        <v>237</v>
+      </c>
+      <c r="AD16" s="6">
+        <v>137</v>
+      </c>
+      <c r="AE16" s="6">
+        <v>3</v>
+      </c>
+      <c r="AF16" s="6">
+        <v>3</v>
+      </c>
+      <c r="AG16" s="6">
+        <v>229</v>
+      </c>
+      <c r="AH16" s="6">
+        <v>5</v>
+      </c>
+      <c r="AI16" s="6">
+        <v>66</v>
+      </c>
+      <c r="AJ16" s="6">
+        <v>117</v>
+      </c>
+      <c r="AK16" s="6">
+        <v>2520</v>
+      </c>
+      <c r="AL16" s="4">
+        <v>1</v>
+      </c>
+      <c r="AM16" s="5">
+        <v>1</v>
+      </c>
+      <c r="AN16" s="5">
+        <v>0.98507460000000002</v>
+      </c>
+      <c r="AO16" s="5">
+        <v>0.3786408</v>
+      </c>
+      <c r="AP16" s="5">
+        <v>0.70806409999999997</v>
+      </c>
+    </row>
+    <row r="17" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="A17" s="9">
+        <v>42887</v>
+      </c>
+      <c r="B17" s="10">
+        <v>229</v>
+      </c>
+      <c r="C17" s="10">
+        <v>5</v>
+      </c>
+      <c r="D17" s="10">
+        <v>309</v>
+      </c>
+      <c r="E17" s="10">
+        <v>67</v>
+      </c>
+      <c r="F17" s="10">
+        <v>3559</v>
+      </c>
+      <c r="G17" s="10">
+        <v>3</v>
+      </c>
+      <c r="H17" s="10">
+        <v>62</v>
+      </c>
+      <c r="I17" s="10">
+        <v>216</v>
+      </c>
+      <c r="J17" s="10">
+        <v>657</v>
+      </c>
+      <c r="K17" s="10">
+        <v>130</v>
+      </c>
+      <c r="L17" s="10">
+        <v>1</v>
+      </c>
+      <c r="M17" s="10">
+        <v>226</v>
+      </c>
+      <c r="N17" s="10">
+        <v>10</v>
+      </c>
+      <c r="O17" s="10">
+        <v>0</v>
+      </c>
+      <c r="P17" s="10">
+        <v>10</v>
+      </c>
+      <c r="Q17" s="10">
+        <v>85</v>
+      </c>
+      <c r="R17" s="10">
+        <v>15</v>
+      </c>
+      <c r="S17" s="10">
+        <v>1</v>
+      </c>
+      <c r="T17" s="10">
+        <v>7</v>
+      </c>
+      <c r="U17" s="10">
+        <v>7</v>
+      </c>
+      <c r="V17" s="10">
+        <v>83</v>
+      </c>
+      <c r="W17" s="10">
+        <v>18</v>
+      </c>
+      <c r="X17" s="10">
+        <v>15</v>
+      </c>
+      <c r="Y17" s="10">
+        <v>45</v>
+      </c>
+      <c r="Z17" s="10">
+        <v>240</v>
+      </c>
+      <c r="AA17" s="10">
+        <v>130</v>
+      </c>
+      <c r="AB17" s="10">
+        <v>0</v>
+      </c>
+      <c r="AC17" s="10">
+        <v>237</v>
+      </c>
+      <c r="AD17" s="6">
+        <v>137</v>
+      </c>
+      <c r="AE17" s="6">
+        <v>3</v>
+      </c>
+      <c r="AF17" s="6">
+        <v>3</v>
+      </c>
+      <c r="AG17" s="6">
+        <v>229</v>
+      </c>
+      <c r="AH17" s="6">
+        <v>5</v>
+      </c>
+      <c r="AI17" s="6">
+        <v>66</v>
+      </c>
+      <c r="AJ17" s="6">
+        <v>117</v>
+      </c>
+      <c r="AK17" s="6">
+        <v>2520</v>
+      </c>
+      <c r="AL17" s="4">
+        <v>1</v>
+      </c>
+      <c r="AM17" s="5">
+        <v>1</v>
+      </c>
+      <c r="AN17" s="5">
+        <v>0.98507460000000002</v>
+      </c>
+      <c r="AO17" s="5">
+        <v>0.3786408</v>
+      </c>
+      <c r="AP17" s="5">
+        <v>0.70806409999999997</v>
+      </c>
+    </row>
+    <row r="18" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="A18" s="9">
+        <v>42888</v>
+      </c>
+      <c r="B18" s="10">
+        <v>229</v>
+      </c>
+      <c r="C18" s="10">
+        <v>5</v>
+      </c>
+      <c r="D18" s="10">
+        <v>309</v>
+      </c>
+      <c r="E18" s="10">
+        <v>67</v>
+      </c>
+      <c r="F18" s="10">
+        <v>3559</v>
+      </c>
+      <c r="G18" s="10">
+        <v>3</v>
+      </c>
+      <c r="H18" s="10">
+        <v>62</v>
+      </c>
+      <c r="I18" s="10">
+        <v>216</v>
+      </c>
+      <c r="J18" s="10">
+        <v>657</v>
+      </c>
+      <c r="K18" s="10">
+        <v>130</v>
+      </c>
+      <c r="L18" s="10">
+        <v>1</v>
+      </c>
+      <c r="M18" s="10">
+        <v>226</v>
+      </c>
+      <c r="N18" s="10">
+        <v>10</v>
+      </c>
+      <c r="O18" s="10">
+        <v>0</v>
+      </c>
+      <c r="P18" s="10">
+        <v>10</v>
+      </c>
+      <c r="Q18" s="10">
+        <v>85</v>
+      </c>
+      <c r="R18" s="10">
+        <v>15</v>
+      </c>
+      <c r="S18" s="10">
+        <v>1</v>
+      </c>
+      <c r="T18" s="10">
+        <v>7</v>
+      </c>
+      <c r="U18" s="10">
+        <v>7</v>
+      </c>
+      <c r="V18" s="10">
+        <v>83</v>
+      </c>
+      <c r="W18" s="10">
+        <v>18</v>
+      </c>
+      <c r="X18" s="10">
+        <v>15</v>
+      </c>
+      <c r="Y18" s="10">
+        <v>45</v>
+      </c>
+      <c r="Z18" s="10">
+        <v>240</v>
+      </c>
+      <c r="AA18" s="10">
+        <v>130</v>
+      </c>
+      <c r="AB18" s="10">
+        <v>0</v>
+      </c>
+      <c r="AC18" s="10">
+        <v>237</v>
+      </c>
+      <c r="AD18" s="6">
+        <v>137</v>
+      </c>
+      <c r="AE18" s="6">
+        <v>3</v>
+      </c>
+      <c r="AF18" s="6">
+        <v>3</v>
+      </c>
+      <c r="AG18" s="6">
+        <v>229</v>
+      </c>
+      <c r="AH18" s="6">
+        <v>5</v>
+      </c>
+      <c r="AI18" s="6">
+        <v>66</v>
+      </c>
+      <c r="AJ18" s="6">
+        <v>117</v>
+      </c>
+      <c r="AK18" s="6">
+        <v>2520</v>
+      </c>
+      <c r="AL18" s="4">
+        <v>1</v>
+      </c>
+      <c r="AM18" s="5">
+        <v>1</v>
+      </c>
+      <c r="AN18" s="5">
+        <v>0.98507460000000002</v>
+      </c>
+      <c r="AO18" s="5">
+        <v>0.3786408</v>
+      </c>
+      <c r="AP18" s="5">
+        <v>0.70806409999999997</v>
+      </c>
+    </row>
+    <row r="19" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="A19" s="9">
+        <v>42891</v>
+      </c>
+      <c r="B19" s="10">
+        <v>231</v>
+      </c>
+      <c r="C19" s="10">
+        <v>5</v>
+      </c>
+      <c r="D19" s="10">
+        <v>309</v>
+      </c>
+      <c r="E19" s="10">
+        <v>67</v>
+      </c>
+      <c r="F19" s="10">
+        <v>3559</v>
+      </c>
+      <c r="G19" s="11">
+        <v>0</v>
+      </c>
+      <c r="H19" s="10">
+        <v>62</v>
+      </c>
+      <c r="I19" s="10">
+        <v>216</v>
+      </c>
+      <c r="J19" s="10">
+        <v>657</v>
+      </c>
+      <c r="K19" s="10">
+        <v>130</v>
+      </c>
+      <c r="L19" s="11">
+        <v>0</v>
+      </c>
+      <c r="M19" s="11">
+        <v>228</v>
+      </c>
+      <c r="N19" s="10">
+        <v>10</v>
+      </c>
+      <c r="O19" s="10">
+        <v>0</v>
+      </c>
+      <c r="P19" s="10">
+        <v>10</v>
+      </c>
+      <c r="Q19" s="11">
+        <v>82</v>
+      </c>
+      <c r="R19" s="11">
+        <v>1</v>
+      </c>
+      <c r="S19" s="11">
+        <v>0</v>
+      </c>
+      <c r="T19" s="11">
+        <v>1</v>
+      </c>
+      <c r="U19" s="11">
+        <v>0</v>
+      </c>
+      <c r="V19" s="12">
+        <v>84</v>
+      </c>
+      <c r="W19" s="10">
+        <v>18</v>
+      </c>
+      <c r="X19" s="10">
+        <v>15</v>
+      </c>
+      <c r="Y19" s="10">
+        <v>45</v>
+      </c>
+      <c r="Z19" s="10">
+        <v>240</v>
+      </c>
+      <c r="AA19" s="10">
+        <v>130</v>
+      </c>
+      <c r="AB19" s="10">
+        <v>0</v>
+      </c>
+      <c r="AC19" s="11">
+        <v>370</v>
+      </c>
+      <c r="AD19" s="11">
+        <v>0</v>
+      </c>
+      <c r="AE19" s="13">
+        <v>1</v>
+      </c>
+      <c r="AF19" s="6">
+        <v>3</v>
+      </c>
+      <c r="AG19" s="13">
+        <v>231</v>
+      </c>
+      <c r="AH19" s="6">
+        <v>5</v>
+      </c>
+      <c r="AI19" s="6">
+        <v>66</v>
+      </c>
+      <c r="AJ19" s="6">
+        <v>117</v>
+      </c>
+      <c r="AK19" s="13">
+        <v>2525</v>
+      </c>
+      <c r="AL19" s="14">
+        <v>1</v>
+      </c>
+      <c r="AM19" s="4">
+        <v>1</v>
+      </c>
+      <c r="AN19" s="5">
+        <v>0.98507460000000002</v>
+      </c>
+      <c r="AO19" s="5">
+        <v>0.3786408</v>
+      </c>
+      <c r="AP19" s="5">
+        <v>0.70946900000000002</v>
+      </c>
+      <c r="AQ19" s="5"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
SNAPSHOT_v11.1d_2017-06-06. Updated metrics spreadsheet. Added SmartClient files to make GitHub pages work.
</commit_message>
<xml_diff>
--- a/referenceDocsMetrics.xlsx
+++ b/referenceDocsMetrics.xlsx
@@ -333,10 +333,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$A$2:$A$19</c:f>
+              <c:f>Sheet1!$A$2:$A$20</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="18"/>
+                <c:ptCount val="19"/>
                 <c:pt idx="0">
                   <c:v>42864</c:v>
                 </c:pt>
@@ -390,16 +390,19 @@
                 </c:pt>
                 <c:pt idx="17">
                   <c:v>42891</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>42892</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$G$2:$G$19</c:f>
+              <c:f>Sheet1!$G$2:$G$20</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="18"/>
+                <c:ptCount val="19"/>
                 <c:pt idx="0">
                   <c:v>3</c:v>
                 </c:pt>
@@ -452,6 +455,9 @@
                   <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="17">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="18">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -478,10 +484,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$A$2:$A$19</c:f>
+              <c:f>Sheet1!$A$2:$A$20</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="18"/>
+                <c:ptCount val="19"/>
                 <c:pt idx="0">
                   <c:v>42864</c:v>
                 </c:pt>
@@ -535,16 +541,19 @@
                 </c:pt>
                 <c:pt idx="17">
                   <c:v>42891</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>42892</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$H$2:$H$19</c:f>
+              <c:f>Sheet1!$H$2:$H$20</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="18"/>
+                <c:ptCount val="19"/>
                 <c:pt idx="0">
                   <c:v>202</c:v>
                 </c:pt>
@@ -597,6 +606,9 @@
                   <c:v>62</c:v>
                 </c:pt>
                 <c:pt idx="17">
+                  <c:v>62</c:v>
+                </c:pt>
+                <c:pt idx="18">
                   <c:v>62</c:v>
                 </c:pt>
               </c:numCache>
@@ -623,10 +635,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$A$2:$A$19</c:f>
+              <c:f>Sheet1!$A$2:$A$20</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="18"/>
+                <c:ptCount val="19"/>
                 <c:pt idx="0">
                   <c:v>42864</c:v>
                 </c:pt>
@@ -680,16 +692,19 @@
                 </c:pt>
                 <c:pt idx="17">
                   <c:v>42891</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>42892</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$I$2:$I$19</c:f>
+              <c:f>Sheet1!$I$2:$I$20</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="18"/>
+                <c:ptCount val="19"/>
                 <c:pt idx="0">
                   <c:v>216</c:v>
                 </c:pt>
@@ -744,295 +759,8 @@
                 <c:pt idx="17">
                   <c:v>216</c:v>
                 </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:ser>
-          <c:idx val="3"/>
-          <c:order val="3"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Sheet1!$J$1</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>string values without quotes</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:cat>
-            <c:numRef>
-              <c:f>Sheet1!$A$2:$A$19</c:f>
-              <c:numCache>
-                <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="18"/>
-                <c:pt idx="0">
-                  <c:v>42864</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>42865</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>42867</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>42868</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>42869</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>42870</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>42872</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>42873</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>42874</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>42875</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>42876</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>42878</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>42880</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>42884</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>42885</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>42887</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>42888</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>42891</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Sheet1!$J$2:$J$19</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="18"/>
-                <c:pt idx="0">
-                  <c:v>657</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>657</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>657</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>657</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>657</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>657</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>657</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>657</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>657</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>657</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>657</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>657</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>657</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>657</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>657</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>657</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>657</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>657</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:ser>
-          <c:idx val="4"/>
-          <c:order val="4"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Sheet1!$K$1</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>string values with period</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:cat>
-            <c:numRef>
-              <c:f>Sheet1!$A$2:$A$19</c:f>
-              <c:numCache>
-                <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="18"/>
-                <c:pt idx="0">
-                  <c:v>42864</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>42865</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>42867</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>42868</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>42869</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>42870</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>42872</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>42873</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>42874</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>42875</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>42876</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>42878</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>42880</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>42884</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>42885</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>42887</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>42888</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>42891</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Sheet1!$K$2:$K$19</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="18"/>
-                <c:pt idx="0">
-                  <c:v>130</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>130</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>130</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>130</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>130</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>130</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>130</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>130</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>130</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>130</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>130</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>130</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>130</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>130</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>130</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>130</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>130</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>130</c:v>
+                <c:pt idx="18">
+                  <c:v>216</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1049,11 +777,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="67624960"/>
-        <c:axId val="67626496"/>
+        <c:axId val="67020288"/>
+        <c:axId val="67021824"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="67624960"/>
+        <c:axId val="67020288"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1063,14 +791,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="67626496"/>
+        <c:crossAx val="67021824"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="67626496"/>
+        <c:axId val="67021824"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1081,7 +809,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="67624960"/>
+        <c:crossAx val="67020288"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1152,10 +880,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$A$2:$A$19</c:f>
+              <c:f>Sheet1!$A$2:$A$20</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="18"/>
+                <c:ptCount val="19"/>
                 <c:pt idx="0">
                   <c:v>42864</c:v>
                 </c:pt>
@@ -1209,16 +937,19 @@
                 </c:pt>
                 <c:pt idx="17">
                   <c:v>42891</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>42892</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$AL$2:$AL$19</c:f>
+              <c:f>Sheet1!$AL$2:$AL$20</c:f>
               <c:numCache>
                 <c:formatCode>0%</c:formatCode>
-                <c:ptCount val="18"/>
+                <c:ptCount val="19"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -1271,6 +1002,9 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="17">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="18">
                   <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
@@ -1297,10 +1031,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$A$2:$A$19</c:f>
+              <c:f>Sheet1!$A$2:$A$20</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="18"/>
+                <c:ptCount val="19"/>
                 <c:pt idx="0">
                   <c:v>42864</c:v>
                 </c:pt>
@@ -1354,16 +1088,19 @@
                 </c:pt>
                 <c:pt idx="17">
                   <c:v>42891</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>42892</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$AM$2:$AM$19</c:f>
+              <c:f>Sheet1!$AM$2:$AM$20</c:f>
               <c:numCache>
                 <c:formatCode>0%</c:formatCode>
-                <c:ptCount val="18"/>
+                <c:ptCount val="19"/>
                 <c:pt idx="0">
                   <c:v>0.6</c:v>
                 </c:pt>
@@ -1416,6 +1153,9 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="17">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="18">
                   <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
@@ -1442,10 +1182,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$A$2:$A$19</c:f>
+              <c:f>Sheet1!$A$2:$A$20</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="18"/>
+                <c:ptCount val="19"/>
                 <c:pt idx="0">
                   <c:v>42864</c:v>
                 </c:pt>
@@ -1499,16 +1239,19 @@
                 </c:pt>
                 <c:pt idx="17">
                   <c:v>42891</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>42892</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$AN$2:$AN$19</c:f>
+              <c:f>Sheet1!$AN$2:$AN$20</c:f>
               <c:numCache>
                 <c:formatCode>0%</c:formatCode>
-                <c:ptCount val="18"/>
+                <c:ptCount val="19"/>
                 <c:pt idx="0">
                   <c:v>0.37313429999999997</c:v>
                 </c:pt>
@@ -1561,6 +1304,9 @@
                   <c:v>0.98507460000000002</c:v>
                 </c:pt>
                 <c:pt idx="17">
+                  <c:v>0.98507460000000002</c:v>
+                </c:pt>
+                <c:pt idx="18">
                   <c:v>0.98507460000000002</c:v>
                 </c:pt>
               </c:numCache>
@@ -1587,10 +1333,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$A$2:$A$19</c:f>
+              <c:f>Sheet1!$A$2:$A$20</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="18"/>
+                <c:ptCount val="19"/>
                 <c:pt idx="0">
                   <c:v>42864</c:v>
                 </c:pt>
@@ -1644,16 +1390,19 @@
                 </c:pt>
                 <c:pt idx="17">
                   <c:v>42891</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>42892</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$AO$2:$AO$19</c:f>
+              <c:f>Sheet1!$AO$2:$AO$20</c:f>
               <c:numCache>
                 <c:formatCode>0%</c:formatCode>
-                <c:ptCount val="18"/>
+                <c:ptCount val="19"/>
                 <c:pt idx="0">
                   <c:v>0.24919089999999999</c:v>
                 </c:pt>
@@ -1706,6 +1455,9 @@
                   <c:v>0.3786408</c:v>
                 </c:pt>
                 <c:pt idx="17">
+                  <c:v>0.3786408</c:v>
+                </c:pt>
+                <c:pt idx="18">
                   <c:v>0.3786408</c:v>
                 </c:pt>
               </c:numCache>
@@ -1732,10 +1484,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$A$2:$A$19</c:f>
+              <c:f>Sheet1!$A$2:$A$20</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="18"/>
+                <c:ptCount val="19"/>
                 <c:pt idx="0">
                   <c:v>42864</c:v>
                 </c:pt>
@@ -1789,16 +1541,19 @@
                 </c:pt>
                 <c:pt idx="17">
                   <c:v>42891</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>42892</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$AP$2:$AP$19</c:f>
+              <c:f>Sheet1!$AP$2:$AP$20</c:f>
               <c:numCache>
                 <c:formatCode>0%</c:formatCode>
-                <c:ptCount val="18"/>
+                <c:ptCount val="19"/>
                 <c:pt idx="0">
                   <c:v>9.9296759999999998E-2</c:v>
                 </c:pt>
@@ -1852,6 +1607,9 @@
                 </c:pt>
                 <c:pt idx="17">
                   <c:v>0.70946900000000002</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.70955060000000003</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1868,11 +1626,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="73884032"/>
-        <c:axId val="73885568"/>
+        <c:axId val="67041152"/>
+        <c:axId val="67042688"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="73884032"/>
+        <c:axId val="67041152"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1882,14 +1640,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="73885568"/>
+        <c:crossAx val="67042688"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="73885568"/>
+        <c:axId val="67042688"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1900,7 +1658,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="73884032"/>
+        <c:crossAx val="67041152"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1928,13 +1686,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>257175</xdr:colOff>
-      <xdr:row>30</xdr:row>
+      <xdr:row>29</xdr:row>
       <xdr:rowOff>9524</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
       <xdr:colOff>95250</xdr:colOff>
-      <xdr:row>53</xdr:row>
+      <xdr:row>52</xdr:row>
       <xdr:rowOff>171449</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -1958,13 +1716,13 @@
     <xdr:from>
       <xdr:col>16</xdr:col>
       <xdr:colOff>466725</xdr:colOff>
-      <xdr:row>30</xdr:row>
+      <xdr:row>29</xdr:row>
       <xdr:rowOff>28575</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>26</xdr:col>
       <xdr:colOff>600075</xdr:colOff>
-      <xdr:row>54</xdr:row>
+      <xdr:row>53</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -2276,10 +2034,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AQ19"/>
+  <dimension ref="A1:AQ20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="X1" workbookViewId="0">
-      <selection activeCell="Q19" sqref="Q19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M25" sqref="M25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4733,6 +4491,134 @@
       </c>
       <c r="AQ19" s="5"/>
     </row>
+    <row r="20" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="A20" s="9">
+        <v>42892</v>
+      </c>
+      <c r="B20" s="10">
+        <v>231</v>
+      </c>
+      <c r="C20" s="10">
+        <v>5</v>
+      </c>
+      <c r="D20" s="10">
+        <v>309</v>
+      </c>
+      <c r="E20" s="10">
+        <v>67</v>
+      </c>
+      <c r="F20" s="10">
+        <v>3560</v>
+      </c>
+      <c r="G20" s="10">
+        <v>0</v>
+      </c>
+      <c r="H20" s="10">
+        <v>62</v>
+      </c>
+      <c r="I20" s="10">
+        <v>216</v>
+      </c>
+      <c r="J20" s="10">
+        <v>657</v>
+      </c>
+      <c r="K20" s="10">
+        <v>130</v>
+      </c>
+      <c r="L20" s="10">
+        <v>0</v>
+      </c>
+      <c r="M20" s="11">
+        <v>238</v>
+      </c>
+      <c r="N20" s="11">
+        <v>0</v>
+      </c>
+      <c r="O20" s="10">
+        <v>0</v>
+      </c>
+      <c r="P20" s="10">
+        <v>10</v>
+      </c>
+      <c r="Q20" s="10">
+        <v>82</v>
+      </c>
+      <c r="R20" s="10">
+        <v>1</v>
+      </c>
+      <c r="S20" s="10">
+        <v>0</v>
+      </c>
+      <c r="T20" s="10">
+        <v>1</v>
+      </c>
+      <c r="U20" s="10">
+        <v>0</v>
+      </c>
+      <c r="V20" s="10">
+        <v>84</v>
+      </c>
+      <c r="W20" s="10">
+        <v>18</v>
+      </c>
+      <c r="X20" s="10">
+        <v>15</v>
+      </c>
+      <c r="Y20" s="10">
+        <v>45</v>
+      </c>
+      <c r="Z20" s="10">
+        <v>240</v>
+      </c>
+      <c r="AA20" s="10">
+        <v>130</v>
+      </c>
+      <c r="AB20" s="10">
+        <v>0</v>
+      </c>
+      <c r="AC20" s="10">
+        <v>370</v>
+      </c>
+      <c r="AD20" s="6">
+        <v>0</v>
+      </c>
+      <c r="AE20" s="6">
+        <v>1</v>
+      </c>
+      <c r="AF20" s="6">
+        <v>3</v>
+      </c>
+      <c r="AG20" s="6">
+        <v>231</v>
+      </c>
+      <c r="AH20" s="6">
+        <v>5</v>
+      </c>
+      <c r="AI20" s="6">
+        <v>66</v>
+      </c>
+      <c r="AJ20" s="6">
+        <v>117</v>
+      </c>
+      <c r="AK20" s="13">
+        <v>2526</v>
+      </c>
+      <c r="AL20" s="4">
+        <v>1</v>
+      </c>
+      <c r="AM20" s="5">
+        <v>1</v>
+      </c>
+      <c r="AN20" s="5">
+        <v>0.98507460000000002</v>
+      </c>
+      <c r="AO20" s="5">
+        <v>0.3786408</v>
+      </c>
+      <c r="AP20" s="5">
+        <v>0.70955060000000003</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Updated with latest. Looking good.
</commit_message>
<xml_diff>
--- a/referenceDocsMetrics.xlsx
+++ b/referenceDocsMetrics.xlsx
@@ -232,7 +232,7 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -274,6 +274,9 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="4" fillId="3" borderId="0" xfId="3" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -333,10 +336,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$A$2:$A$20</c:f>
+              <c:f>Sheet1!$A$2:$A$21</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="19"/>
+                <c:ptCount val="20"/>
                 <c:pt idx="0">
                   <c:v>42864</c:v>
                 </c:pt>
@@ -393,16 +396,19 @@
                 </c:pt>
                 <c:pt idx="18">
                   <c:v>42892</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>42893</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$G$2:$G$20</c:f>
+              <c:f>Sheet1!$G$2:$G$21</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="19"/>
+                <c:ptCount val="20"/>
                 <c:pt idx="0">
                   <c:v>3</c:v>
                 </c:pt>
@@ -458,6 +464,9 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="18">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="19">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -484,10 +493,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$A$2:$A$20</c:f>
+              <c:f>Sheet1!$A$2:$A$21</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="19"/>
+                <c:ptCount val="20"/>
                 <c:pt idx="0">
                   <c:v>42864</c:v>
                 </c:pt>
@@ -544,16 +553,19 @@
                 </c:pt>
                 <c:pt idx="18">
                   <c:v>42892</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>42893</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$H$2:$H$20</c:f>
+              <c:f>Sheet1!$H$2:$H$21</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="19"/>
+                <c:ptCount val="20"/>
                 <c:pt idx="0">
                   <c:v>202</c:v>
                 </c:pt>
@@ -609,6 +621,9 @@
                   <c:v>62</c:v>
                 </c:pt>
                 <c:pt idx="18">
+                  <c:v>62</c:v>
+                </c:pt>
+                <c:pt idx="19">
                   <c:v>62</c:v>
                 </c:pt>
               </c:numCache>
@@ -635,10 +650,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$A$2:$A$20</c:f>
+              <c:f>Sheet1!$A$2:$A$21</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="19"/>
+                <c:ptCount val="20"/>
                 <c:pt idx="0">
                   <c:v>42864</c:v>
                 </c:pt>
@@ -695,16 +710,19 @@
                 </c:pt>
                 <c:pt idx="18">
                   <c:v>42892</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>42893</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$I$2:$I$20</c:f>
+              <c:f>Sheet1!$I$2:$I$21</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="19"/>
+                <c:ptCount val="20"/>
                 <c:pt idx="0">
                   <c:v>216</c:v>
                 </c:pt>
@@ -760,6 +778,9 @@
                   <c:v>216</c:v>
                 </c:pt>
                 <c:pt idx="18">
+                  <c:v>216</c:v>
+                </c:pt>
+                <c:pt idx="19">
                   <c:v>216</c:v>
                 </c:pt>
               </c:numCache>
@@ -777,11 +798,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="67020288"/>
-        <c:axId val="67021824"/>
+        <c:axId val="101625216"/>
+        <c:axId val="40252544"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="67020288"/>
+        <c:axId val="101625216"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -791,14 +812,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="67021824"/>
+        <c:crossAx val="40252544"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="67021824"/>
+        <c:axId val="40252544"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -809,7 +830,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="67020288"/>
+        <c:crossAx val="101625216"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -880,10 +901,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$A$2:$A$20</c:f>
+              <c:f>Sheet1!$A$2:$A$21</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="19"/>
+                <c:ptCount val="20"/>
                 <c:pt idx="0">
                   <c:v>42864</c:v>
                 </c:pt>
@@ -940,16 +961,19 @@
                 </c:pt>
                 <c:pt idx="18">
                   <c:v>42892</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>42893</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$AL$2:$AL$20</c:f>
+              <c:f>Sheet1!$AL$2:$AL$21</c:f>
               <c:numCache>
                 <c:formatCode>0%</c:formatCode>
-                <c:ptCount val="19"/>
+                <c:ptCount val="20"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -1005,6 +1029,9 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="18">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="19">
                   <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
@@ -1031,10 +1058,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$A$2:$A$20</c:f>
+              <c:f>Sheet1!$A$2:$A$21</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="19"/>
+                <c:ptCount val="20"/>
                 <c:pt idx="0">
                   <c:v>42864</c:v>
                 </c:pt>
@@ -1091,16 +1118,19 @@
                 </c:pt>
                 <c:pt idx="18">
                   <c:v>42892</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>42893</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$AM$2:$AM$20</c:f>
+              <c:f>Sheet1!$AM$2:$AM$21</c:f>
               <c:numCache>
                 <c:formatCode>0%</c:formatCode>
-                <c:ptCount val="19"/>
+                <c:ptCount val="20"/>
                 <c:pt idx="0">
                   <c:v>0.6</c:v>
                 </c:pt>
@@ -1156,6 +1186,9 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="18">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="19">
                   <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
@@ -1182,10 +1215,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$A$2:$A$20</c:f>
+              <c:f>Sheet1!$A$2:$A$21</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="19"/>
+                <c:ptCount val="20"/>
                 <c:pt idx="0">
                   <c:v>42864</c:v>
                 </c:pt>
@@ -1242,16 +1275,19 @@
                 </c:pt>
                 <c:pt idx="18">
                   <c:v>42892</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>42893</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$AN$2:$AN$20</c:f>
+              <c:f>Sheet1!$AN$2:$AN$21</c:f>
               <c:numCache>
                 <c:formatCode>0%</c:formatCode>
-                <c:ptCount val="19"/>
+                <c:ptCount val="20"/>
                 <c:pt idx="0">
                   <c:v>0.37313429999999997</c:v>
                 </c:pt>
@@ -1307,6 +1343,9 @@
                   <c:v>0.98507460000000002</c:v>
                 </c:pt>
                 <c:pt idx="18">
+                  <c:v>0.98507460000000002</c:v>
+                </c:pt>
+                <c:pt idx="19">
                   <c:v>0.98507460000000002</c:v>
                 </c:pt>
               </c:numCache>
@@ -1333,10 +1372,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$A$2:$A$20</c:f>
+              <c:f>Sheet1!$A$2:$A$21</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="19"/>
+                <c:ptCount val="20"/>
                 <c:pt idx="0">
                   <c:v>42864</c:v>
                 </c:pt>
@@ -1393,16 +1432,19 @@
                 </c:pt>
                 <c:pt idx="18">
                   <c:v>42892</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>42893</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$AO$2:$AO$20</c:f>
+              <c:f>Sheet1!$AO$2:$AO$21</c:f>
               <c:numCache>
                 <c:formatCode>0%</c:formatCode>
-                <c:ptCount val="19"/>
+                <c:ptCount val="20"/>
                 <c:pt idx="0">
                   <c:v>0.24919089999999999</c:v>
                 </c:pt>
@@ -1458,6 +1500,9 @@
                   <c:v>0.3786408</c:v>
                 </c:pt>
                 <c:pt idx="18">
+                  <c:v>0.3786408</c:v>
+                </c:pt>
+                <c:pt idx="19">
                   <c:v>0.3786408</c:v>
                 </c:pt>
               </c:numCache>
@@ -1484,10 +1529,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$A$2:$A$20</c:f>
+              <c:f>Sheet1!$A$2:$A$21</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="19"/>
+                <c:ptCount val="20"/>
                 <c:pt idx="0">
                   <c:v>42864</c:v>
                 </c:pt>
@@ -1544,16 +1589,19 @@
                 </c:pt>
                 <c:pt idx="18">
                   <c:v>42892</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>42893</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$AP$2:$AP$20</c:f>
+              <c:f>Sheet1!$AP$2:$AP$21</c:f>
               <c:numCache>
                 <c:formatCode>0%</c:formatCode>
-                <c:ptCount val="19"/>
+                <c:ptCount val="20"/>
                 <c:pt idx="0">
                   <c:v>9.9296759999999998E-2</c:v>
                 </c:pt>
@@ -1610,6 +1658,9 @@
                 </c:pt>
                 <c:pt idx="18">
                   <c:v>0.70955060000000003</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.72528090000000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1626,11 +1677,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="67041152"/>
-        <c:axId val="67042688"/>
+        <c:axId val="67031040"/>
+        <c:axId val="67032576"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="67041152"/>
+        <c:axId val="67031040"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1640,14 +1691,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="67042688"/>
+        <c:crossAx val="67032576"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="67042688"/>
+        <c:axId val="67032576"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1658,7 +1709,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="67041152"/>
+        <c:crossAx val="67031040"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2034,10 +2085,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AQ20"/>
+  <dimension ref="A1:AQ21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M25" sqref="M25"/>
+      <selection activeCell="AP21" sqref="AP21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4619,6 +4670,134 @@
         <v>0.70955060000000003</v>
       </c>
     </row>
+    <row r="21" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="A21" s="9">
+        <v>42893</v>
+      </c>
+      <c r="B21" s="10">
+        <v>231</v>
+      </c>
+      <c r="C21" s="10">
+        <v>5</v>
+      </c>
+      <c r="D21" s="10">
+        <v>309</v>
+      </c>
+      <c r="E21" s="10">
+        <v>67</v>
+      </c>
+      <c r="F21" s="10">
+        <v>3560</v>
+      </c>
+      <c r="G21" s="10">
+        <v>0</v>
+      </c>
+      <c r="H21" s="10">
+        <v>62</v>
+      </c>
+      <c r="I21" s="10">
+        <v>216</v>
+      </c>
+      <c r="J21" s="10">
+        <v>657</v>
+      </c>
+      <c r="K21" s="10">
+        <v>130</v>
+      </c>
+      <c r="L21" s="10">
+        <v>0</v>
+      </c>
+      <c r="M21" s="11">
+        <v>239</v>
+      </c>
+      <c r="N21" s="10">
+        <v>0</v>
+      </c>
+      <c r="O21" s="10">
+        <v>0</v>
+      </c>
+      <c r="P21" s="11">
+        <v>8</v>
+      </c>
+      <c r="Q21" s="12">
+        <v>83</v>
+      </c>
+      <c r="R21" s="10">
+        <v>1</v>
+      </c>
+      <c r="S21" s="10">
+        <v>0</v>
+      </c>
+      <c r="T21" s="10">
+        <v>1</v>
+      </c>
+      <c r="U21" s="10">
+        <v>0</v>
+      </c>
+      <c r="V21" s="11">
+        <v>12</v>
+      </c>
+      <c r="W21" s="10">
+        <v>18</v>
+      </c>
+      <c r="X21" s="11">
+        <v>1</v>
+      </c>
+      <c r="Y21" s="10">
+        <v>45</v>
+      </c>
+      <c r="Z21" s="10">
+        <v>240</v>
+      </c>
+      <c r="AA21" s="10">
+        <v>130</v>
+      </c>
+      <c r="AB21" s="10">
+        <v>0</v>
+      </c>
+      <c r="AC21" s="11">
+        <v>374</v>
+      </c>
+      <c r="AD21" s="6">
+        <v>0</v>
+      </c>
+      <c r="AE21" s="6">
+        <v>1</v>
+      </c>
+      <c r="AF21" s="6">
+        <v>3</v>
+      </c>
+      <c r="AG21" s="6">
+        <v>231</v>
+      </c>
+      <c r="AH21" s="6">
+        <v>5</v>
+      </c>
+      <c r="AI21" s="6">
+        <v>66</v>
+      </c>
+      <c r="AJ21" s="6">
+        <v>117</v>
+      </c>
+      <c r="AK21" s="13">
+        <v>2582</v>
+      </c>
+      <c r="AL21" s="4">
+        <v>1</v>
+      </c>
+      <c r="AM21" s="5">
+        <v>1</v>
+      </c>
+      <c r="AN21" s="5">
+        <v>0.98507460000000002</v>
+      </c>
+      <c r="AO21" s="5">
+        <v>0.3786408</v>
+      </c>
+      <c r="AP21" s="15">
+        <v>0.72528090000000001</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Updated metrics to 2017-06-15
</commit_message>
<xml_diff>
--- a/referenceDocsMetrics.xlsx
+++ b/referenceDocsMetrics.xlsx
@@ -330,7 +330,17 @@
   <c:chart>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="4.4879498522554531E-2"/>
+          <c:y val="3.1034296813527242E-2"/>
+          <c:w val="0.93466354666621121"/>
+          <c:h val="0.82352630449495701"/>
+        </c:manualLayout>
+      </c:layout>
       <c:lineChart>
         <c:grouping val="standard"/>
         <c:varyColors val="0"/>
@@ -353,10 +363,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$A$2:$A$26</c:f>
+              <c:f>Sheet1!$A$2:$A$27</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="25"/>
+                <c:ptCount val="26"/>
                 <c:pt idx="0">
                   <c:v>42864</c:v>
                 </c:pt>
@@ -431,16 +441,19 @@
                 </c:pt>
                 <c:pt idx="24">
                   <c:v>42900</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>42901</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$G$2:$G$26</c:f>
+              <c:f>Sheet1!$G$2:$G$27</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="25"/>
+                <c:ptCount val="26"/>
                 <c:pt idx="0">
                   <c:v>3</c:v>
                 </c:pt>
@@ -514,6 +527,9 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="24">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="25">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -540,10 +556,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$A$2:$A$26</c:f>
+              <c:f>Sheet1!$A$2:$A$27</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="25"/>
+                <c:ptCount val="26"/>
                 <c:pt idx="0">
                   <c:v>42864</c:v>
                 </c:pt>
@@ -618,16 +634,19 @@
                 </c:pt>
                 <c:pt idx="24">
                   <c:v>42900</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>42901</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$H$2:$H$26</c:f>
+              <c:f>Sheet1!$H$2:$H$27</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="25"/>
+                <c:ptCount val="26"/>
                 <c:pt idx="0">
                   <c:v>202</c:v>
                 </c:pt>
@@ -702,6 +721,9 @@
                 </c:pt>
                 <c:pt idx="24">
                   <c:v>62</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>61</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -727,10 +749,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$A$2:$A$26</c:f>
+              <c:f>Sheet1!$A$2:$A$27</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="25"/>
+                <c:ptCount val="26"/>
                 <c:pt idx="0">
                   <c:v>42864</c:v>
                 </c:pt>
@@ -805,16 +827,19 @@
                 </c:pt>
                 <c:pt idx="24">
                   <c:v>42900</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>42901</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$I$2:$I$26</c:f>
+              <c:f>Sheet1!$I$2:$I$27</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="25"/>
+                <c:ptCount val="26"/>
                 <c:pt idx="0">
                   <c:v>216</c:v>
                 </c:pt>
@@ -888,6 +913,9 @@
                   <c:v>216</c:v>
                 </c:pt>
                 <c:pt idx="24">
+                  <c:v>216</c:v>
+                </c:pt>
+                <c:pt idx="25">
                   <c:v>216</c:v>
                 </c:pt>
               </c:numCache>
@@ -944,7 +972,16 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.73470636127100164"/>
+          <c:y val="0.37107094317612815"/>
+          <c:w val="0.21467903279985881"/>
+          <c:h val="0.15163868667359975"/>
+        </c:manualLayout>
+      </c:layout>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -982,7 +1019,7 @@
           <c:yMode val="edge"/>
           <c:x val="6.5272345295232889E-2"/>
           <c:y val="4.2215289126595022E-2"/>
-          <c:w val="0.67996879999544524"/>
+          <c:w val="0.9084575924755609"/>
           <c:h val="0.82352630449495701"/>
         </c:manualLayout>
       </c:layout>
@@ -1008,10 +1045,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$A$7:$A$26</c:f>
+              <c:f>Sheet1!$A$7:$A$27</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="20"/>
+                <c:ptCount val="21"/>
                 <c:pt idx="0">
                   <c:v>42870</c:v>
                 </c:pt>
@@ -1071,16 +1108,19 @@
                 </c:pt>
                 <c:pt idx="19">
                   <c:v>42900</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>42901</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$AL$7:$AL$26</c:f>
+              <c:f>Sheet1!$AL$7:$AL$27</c:f>
               <c:numCache>
                 <c:formatCode>0%</c:formatCode>
-                <c:ptCount val="20"/>
+                <c:ptCount val="21"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -1139,6 +1179,9 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="19">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="20">
                   <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
@@ -1165,10 +1208,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$A$7:$A$26</c:f>
+              <c:f>Sheet1!$A$7:$A$27</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="20"/>
+                <c:ptCount val="21"/>
                 <c:pt idx="0">
                   <c:v>42870</c:v>
                 </c:pt>
@@ -1228,16 +1271,19 @@
                 </c:pt>
                 <c:pt idx="19">
                   <c:v>42900</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>42901</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$AM$7:$AM$26</c:f>
+              <c:f>Sheet1!$AM$7:$AM$27</c:f>
               <c:numCache>
                 <c:formatCode>0%</c:formatCode>
-                <c:ptCount val="20"/>
+                <c:ptCount val="21"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -1296,6 +1342,9 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="19">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="20">
                   <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
@@ -1322,10 +1371,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$A$7:$A$26</c:f>
+              <c:f>Sheet1!$A$7:$A$27</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="20"/>
+                <c:ptCount val="21"/>
                 <c:pt idx="0">
                   <c:v>42870</c:v>
                 </c:pt>
@@ -1385,16 +1434,19 @@
                 </c:pt>
                 <c:pt idx="19">
                   <c:v>42900</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>42901</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$AN$7:$AN$26</c:f>
+              <c:f>Sheet1!$AN$7:$AN$27</c:f>
               <c:numCache>
                 <c:formatCode>0%</c:formatCode>
-                <c:ptCount val="20"/>
+                <c:ptCount val="21"/>
                 <c:pt idx="0">
                   <c:v>0.59701490000000002</c:v>
                 </c:pt>
@@ -1454,6 +1506,9 @@
                 </c:pt>
                 <c:pt idx="19">
                   <c:v>0.98507460000000002</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.98550720000000003</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1479,10 +1534,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$A$7:$A$26</c:f>
+              <c:f>Sheet1!$A$7:$A$27</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="20"/>
+                <c:ptCount val="21"/>
                 <c:pt idx="0">
                   <c:v>42870</c:v>
                 </c:pt>
@@ -1542,16 +1597,19 @@
                 </c:pt>
                 <c:pt idx="19">
                   <c:v>42900</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>42901</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$AO$7:$AO$26</c:f>
+              <c:f>Sheet1!$AO$7:$AO$27</c:f>
               <c:numCache>
                 <c:formatCode>0%</c:formatCode>
-                <c:ptCount val="20"/>
+                <c:ptCount val="21"/>
                 <c:pt idx="0">
                   <c:v>0.33980579999999999</c:v>
                 </c:pt>
@@ -1611,6 +1669,9 @@
                 </c:pt>
                 <c:pt idx="19">
                   <c:v>0.38511329999999999</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.38110749999999999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1636,10 +1697,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$A$7:$A$26</c:f>
+              <c:f>Sheet1!$A$7:$A$27</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="20"/>
+                <c:ptCount val="21"/>
                 <c:pt idx="0">
                   <c:v>42870</c:v>
                 </c:pt>
@@ -1699,16 +1760,19 @@
                 </c:pt>
                 <c:pt idx="19">
                   <c:v>42900</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>42901</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$AP$7:$AP$26</c:f>
+              <c:f>Sheet1!$AP$7:$AP$27</c:f>
               <c:numCache>
                 <c:formatCode>0%</c:formatCode>
-                <c:ptCount val="20"/>
+                <c:ptCount val="21"/>
                 <c:pt idx="0">
                   <c:v>0.34430379999999999</c:v>
                 </c:pt>
@@ -1768,6 +1832,9 @@
                 </c:pt>
                 <c:pt idx="19">
                   <c:v>0.72668540000000004</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.72688960000000002</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1823,7 +1890,16 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.72549608646162156"/>
+          <c:y val="0.62241150673775836"/>
+          <c:w val="0.25063737965509192"/>
+          <c:h val="0.25273114445599959"/>
+        </c:manualLayout>
+      </c:layout>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1848,8 +1924,8 @@
       <xdr:rowOff>9524</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>95250</xdr:colOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>238125</xdr:colOff>
       <xdr:row>52</xdr:row>
       <xdr:rowOff>171449</xdr:rowOff>
     </xdr:to>
@@ -1872,16 +1948,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>466725</xdr:colOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>400050</xdr:colOff>
       <xdr:row>29</xdr:row>
-      <xdr:rowOff>28575</xdr:rowOff>
+      <xdr:rowOff>47625</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>26</xdr:col>
-      <xdr:colOff>600075</xdr:colOff>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>228600</xdr:colOff>
       <xdr:row>53</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:rowOff>19050</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2192,10 +2268,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AQ26"/>
+  <dimension ref="A1:AQ27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AG26" sqref="AG26"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="W45" sqref="W45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5545,6 +5621,134 @@
         <v>0.72668540000000004</v>
       </c>
     </row>
+    <row r="27" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="A27" s="9">
+        <v>42901</v>
+      </c>
+      <c r="B27" s="10">
+        <v>232</v>
+      </c>
+      <c r="C27" s="10">
+        <v>5</v>
+      </c>
+      <c r="D27" s="11">
+        <v>307</v>
+      </c>
+      <c r="E27" s="11">
+        <v>69</v>
+      </c>
+      <c r="F27" s="16">
+        <v>3559</v>
+      </c>
+      <c r="G27" s="10">
+        <v>0</v>
+      </c>
+      <c r="H27" s="11">
+        <v>61</v>
+      </c>
+      <c r="I27" s="10">
+        <v>216</v>
+      </c>
+      <c r="J27" s="10">
+        <v>657</v>
+      </c>
+      <c r="K27" s="10">
+        <v>130</v>
+      </c>
+      <c r="L27" s="10">
+        <v>0</v>
+      </c>
+      <c r="M27" s="10">
+        <v>239</v>
+      </c>
+      <c r="N27" s="10">
+        <v>0</v>
+      </c>
+      <c r="O27" s="10">
+        <v>0</v>
+      </c>
+      <c r="P27" s="10">
+        <v>8</v>
+      </c>
+      <c r="Q27" s="10">
+        <v>57</v>
+      </c>
+      <c r="R27" s="10">
+        <v>0</v>
+      </c>
+      <c r="S27" s="10">
+        <v>0</v>
+      </c>
+      <c r="T27" s="10">
+        <v>0</v>
+      </c>
+      <c r="U27" s="10">
+        <v>0</v>
+      </c>
+      <c r="V27" s="10">
+        <v>12</v>
+      </c>
+      <c r="W27" s="10">
+        <v>18</v>
+      </c>
+      <c r="X27" s="10">
+        <v>1</v>
+      </c>
+      <c r="Y27" s="10">
+        <v>45</v>
+      </c>
+      <c r="Z27" s="12">
+        <v>283</v>
+      </c>
+      <c r="AA27" s="10">
+        <v>130</v>
+      </c>
+      <c r="AB27" s="10">
+        <v>0</v>
+      </c>
+      <c r="AC27" s="10">
+        <v>379</v>
+      </c>
+      <c r="AD27" s="6">
+        <v>0</v>
+      </c>
+      <c r="AE27" s="6">
+        <v>0</v>
+      </c>
+      <c r="AF27" s="6">
+        <v>3</v>
+      </c>
+      <c r="AG27" s="6">
+        <v>232</v>
+      </c>
+      <c r="AH27" s="6">
+        <v>5</v>
+      </c>
+      <c r="AI27" s="13">
+        <v>68</v>
+      </c>
+      <c r="AJ27" s="13">
+        <v>117</v>
+      </c>
+      <c r="AK27" s="6">
+        <v>2587</v>
+      </c>
+      <c r="AL27" s="4">
+        <v>1</v>
+      </c>
+      <c r="AM27" s="5">
+        <v>1</v>
+      </c>
+      <c r="AN27" s="5">
+        <v>0.98550720000000003</v>
+      </c>
+      <c r="AO27" s="5">
+        <v>0.38110749999999999</v>
+      </c>
+      <c r="AP27" s="5">
+        <v>0.72688960000000002</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>